<commit_message>
Updates on albedo performance.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683DB540-BE02-4362-BC7A-5E1945E364E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6C177F-A2F8-403B-BCA7-84F745D00E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1867,7 +1867,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,20 +2434,44 @@
       <c r="A38" t="s">
         <v>102</v>
       </c>
+      <c r="B38" s="5">
+        <v>14.9251</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0.81540000000000001</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>103</v>
       </c>
+      <c r="B39" s="5">
+        <v>14.056699999999999</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0.69310000000000005</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>104</v>
       </c>
+      <c r="B40" s="5">
+        <v>14.311999999999999</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0.79039999999999999</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>105</v>
+      </c>
+      <c r="B41" s="5">
+        <v>5.6669999999999998</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0.57389999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Checkpoint for shadow relight test.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6C177F-A2F8-403B-BCA7-84F745D00E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4B78E3-3C62-4078-A340-4D5732F783E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
   <si>
     <t>PSNR</t>
   </si>
@@ -450,6 +450,21 @@
   </si>
   <si>
     <t>V7.22.8</t>
+  </si>
+  <si>
+    <t>Shadow Remap</t>
+  </si>
+  <si>
+    <t>V1.02.8</t>
+  </si>
+  <si>
+    <t>V1.02.5</t>
+  </si>
+  <si>
+    <t>V1.02.6</t>
+  </si>
+  <si>
+    <t>V1.02.7</t>
   </si>
 </sst>
 </file>
@@ -557,7 +572,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1797,64 +1832,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="25" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="24" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="23" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="22" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="21" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="20" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="19" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="18" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="17" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="16" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="15" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="14" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="13" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="12" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="11" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="10" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="7" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="6" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1864,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C3ACB0-2CD7-4C40-8065-6A5C0AF1D9C4}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,9 +1915,12 @@
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="5" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1912,8 +1950,17 @@
       <c r="K1" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1932,8 +1979,11 @@
       <c r="G2" s="9">
         <v>0.71689999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1946,8 +1996,11 @@
       <c r="G3" s="9">
         <v>0.71689999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1961,8 +2014,11 @@
         <v>0.7359</v>
       </c>
       <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1975,8 +2031,11 @@
       <c r="G5" s="9">
         <v>0.74690000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2005,7 +2064,7 @@
         <v>0.6835</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2018,7 +2077,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -2037,7 +2096,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2056,7 +2115,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2085,7 +2144,7 @@
         <v>0.76429999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -2104,7 +2163,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -2123,7 +2182,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -2142,7 +2201,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -2171,7 +2230,7 @@
         <v>0.63670000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -2200,7 +2259,7 @@
         <v>0.64510000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -2541,22 +2600,28 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F100">
+    <cfRule type="top10" dxfId="7" priority="11" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G100">
+    <cfRule type="top10" dxfId="6" priority="10" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="top10" dxfId="5" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G100">
+  <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="top10" dxfId="4" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="3" priority="7" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="2" priority="6" percent="1" rank="10"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revised training of maps 2 rgb to make it cyclic
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4B78E3-3C62-4078-A340-4D5732F783E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB231AD6-880B-448E-91E6-F5A64C32F9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId2"/>
+    <sheet name="Maps 2 RGB" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,8 +108,43 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neil Patrick  A. Del Gallego</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{58E97D53-181A-45A8-9A4E-7F9FA955595A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="130">
   <si>
     <t>PSNR</t>
   </si>
@@ -465,6 +501,39 @@
   </si>
   <si>
     <t>V1.02.7</t>
+  </si>
+  <si>
+    <t>V1.01.6</t>
+  </si>
+  <si>
+    <t>V1.01.7</t>
+  </si>
+  <si>
+    <t>V1.01.8</t>
+  </si>
+  <si>
+    <t>Shading</t>
+  </si>
+  <si>
+    <t>Albedo</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>V2.00.5</t>
+  </si>
+  <si>
+    <t>V2.00.6</t>
+  </si>
+  <si>
+    <t>V2.00.7</t>
+  </si>
+  <si>
+    <t>V2.00.8</t>
   </si>
 </sst>
 </file>
@@ -572,7 +641,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1832,64 +2001,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="27" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="26" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="25" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="24" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="23" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="22" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="21" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="20" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="19" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="18" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="17" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="16" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="15" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="14" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="13" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="12" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="9" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="8" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1901,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C3ACB0-2CD7-4C40-8065-6A5C0AF1D9C4}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,8 +2085,8 @@
     <col min="10" max="10" width="12.42578125" style="5" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="5"/>
     <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1980,7 +2149,13 @@
         <v>0.71689999999999998</v>
       </c>
       <c r="M2" t="s">
-        <v>116</v>
+        <v>19</v>
+      </c>
+      <c r="N2" s="5">
+        <v>8.3172999999999995</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.76339999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1997,7 +2172,13 @@
         <v>0.71689999999999998</v>
       </c>
       <c r="M3" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="N3" s="5">
+        <v>10.18</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.76329999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2015,7 +2196,13 @@
       </c>
       <c r="H4" s="7"/>
       <c r="M4" t="s">
-        <v>118</v>
+        <v>120</v>
+      </c>
+      <c r="N4" s="5">
+        <v>8.8404000000000007</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.70250000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2032,7 +2219,13 @@
         <v>0.74690000000000001</v>
       </c>
       <c r="M5" t="s">
-        <v>115</v>
+        <v>121</v>
+      </c>
+      <c r="N5" s="5">
+        <v>7.7416999999999998</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.76100000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2063,6 +2256,15 @@
       <c r="K6" s="9">
         <v>0.6835</v>
       </c>
+      <c r="M6" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="5">
+        <v>7.4988999999999999</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.74399999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2076,6 +2278,15 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
+      <c r="M7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="5">
+        <v>10.4199</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0.81779999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2095,6 +2306,15 @@
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
+      <c r="M8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" s="5">
+        <v>8.4185999999999996</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0.79269999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2114,6 +2334,15 @@
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
+      <c r="M9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N9" s="5">
+        <v>7.5163000000000002</v>
+      </c>
+      <c r="O9" s="5">
+        <v>0.76790000000000003</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2600,27 +2829,193 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F100">
-    <cfRule type="top10" dxfId="7" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G100">
-    <cfRule type="top10" dxfId="6" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="5" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="4" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
+    <cfRule type="top10" dxfId="13" priority="6" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C1048576 C1:C45">
+    <cfRule type="top10" dxfId="12" priority="5" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1">
+    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1">
+    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="top10" dxfId="9" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="top10" dxfId="8" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="9" width="11" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3">
+        <v>17.872399999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.83620000000000005</v>
+      </c>
+      <c r="D3">
+        <v>19.041</v>
+      </c>
+      <c r="E3">
+        <v>0.88360000000000005</v>
+      </c>
+      <c r="F3">
+        <v>16.894400000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.84240000000000004</v>
+      </c>
+      <c r="H3">
+        <v>24.302600000000002</v>
+      </c>
+      <c r="I3">
+        <v>0.9042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>17.502800000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.84709999999999996</v>
+      </c>
+      <c r="D4">
+        <v>19.226800000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.88639999999999997</v>
+      </c>
+      <c r="F4">
+        <v>14.5817</v>
+      </c>
+      <c r="G4">
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="H4">
+        <v>24.2653</v>
+      </c>
+      <c r="I4">
+        <v>0.9103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
     <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:C1048576 C1:C45">
+  <conditionalFormatting sqref="C2">
     <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1">
+  <conditionalFormatting sqref="H2">
     <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1">
+  <conditionalFormatting sqref="I2">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated scripts. Bug fixes and optimization.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B9D998-1171-4697-9328-52CC1BFE3AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AEA069-E711-4E99-A104-26AF2812ECBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="146">
   <si>
     <t>PSNR</t>
   </si>
@@ -567,6 +567,21 @@
   </si>
   <si>
     <t>V1.06.8</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>V1.07.5</t>
+  </si>
+  <si>
+    <t>V1.07.6</t>
+  </si>
+  <si>
+    <t>V1.07.7</t>
+  </si>
+  <si>
+    <t>V1.07.8</t>
   </si>
 </sst>
 </file>
@@ -673,10 +688,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,38 +1415,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="K1" s="12" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="12"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="12"/>
+      <c r="O1" s="13"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2131,7 +2146,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,8 +2348,8 @@
       <c r="E7" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="I7" t="s">
         <v>50</v>
       </c>
@@ -2363,8 +2378,8 @@
       <c r="E8" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
       <c r="I8" t="s">
         <v>51</v>
       </c>
@@ -2393,8 +2408,8 @@
       <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="I9" t="s">
         <v>52</v>
       </c>
@@ -2441,6 +2456,12 @@
       <c r="M10" t="s">
         <v>135</v>
       </c>
+      <c r="N10" s="5">
+        <v>11.668799999999999</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0.78320000000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2463,6 +2484,12 @@
       <c r="M11" t="s">
         <v>134</v>
       </c>
+      <c r="N11" s="5">
+        <v>11.763299999999999</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0.8357</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2485,6 +2512,12 @@
       <c r="M12" t="s">
         <v>136</v>
       </c>
+      <c r="N12" s="5">
+        <v>9.4975000000000005</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0.7722</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2507,6 +2540,12 @@
       <c r="M13" t="s">
         <v>137</v>
       </c>
+      <c r="N13" s="5">
+        <v>10.1137</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0.79610000000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2603,8 +2642,14 @@
       <c r="M16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2623,8 +2668,14 @@
       <c r="M17" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -2640,8 +2691,17 @@
       <c r="I18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>142</v>
+      </c>
+      <c r="N18" s="5">
+        <v>9.3048000000000002</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0.77929999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -2657,8 +2717,17 @@
       <c r="I19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>143</v>
+      </c>
+      <c r="N19" s="5">
+        <v>8.7856000000000005</v>
+      </c>
+      <c r="O19" s="5">
+        <v>0.78190000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -2674,8 +2743,11 @@
       <c r="I20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -2691,8 +2763,11 @@
       <c r="I21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -2712,7 +2787,7 @@
         <v>0.83240000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -2726,7 +2801,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -2746,7 +2821,7 @@
         <v>0.80300000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -2766,7 +2841,7 @@
         <v>0.80479999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2777,7 +2852,7 @@
         <v>0.62780000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -2788,7 +2863,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -2799,7 +2874,7 @@
         <v>0.68899999999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -2810,61 +2885,61 @@
         <v>0.6179</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -3023,7 +3098,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tallied performance from SOTA.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC09F997-D82A-4291-9023-D8AD8AA051AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D870AF2-EEAC-49CF-A102-2A2B19DC3851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId2"/>
     <sheet name="Maps 2 RGB" sheetId="9" r:id="rId3"/>
+    <sheet name="GTA V Images" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -143,8 +144,193 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neil Patrick  A. Del Gallego</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{B4B3E281-9110-47D4-BA31-339CFB884838}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{3A688B25-E717-4102-BC1E-8553E4EEDB4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{E04C5B39-0BFF-49A0-8324-66F643751F79}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{3186612B-4AE9-42BD-9267-7497DCEC16A2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{F57B4E8A-99B3-45C3-8336-732806698F32}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{092728A2-86C5-4AEE-A9AF-BC08FF17E5DA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{4072FB4A-5374-4D7F-8012-AC4E1ADC91AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="162">
   <si>
     <t>PSNR</t>
   </si>
@@ -594,6 +780,42 @@
   </si>
   <si>
     <t>V3.00.8</t>
+  </si>
+  <si>
+    <t>li_eccv18</t>
+  </si>
+  <si>
+    <t>yu_cvpr19</t>
+  </si>
+  <si>
+    <t>yu_eccv20</t>
+  </si>
+  <si>
+    <t>zhu_iccp21</t>
+  </si>
+  <si>
+    <t>Image 1</t>
+  </si>
+  <si>
+    <t>Ours</t>
+  </si>
+  <si>
+    <t>Image 2</t>
+  </si>
+  <si>
+    <t>Image 3</t>
+  </si>
+  <si>
+    <t>Image 4</t>
+  </si>
+  <si>
+    <t>Image 0</t>
+  </si>
+  <si>
+    <t>Image 5</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -708,7 +930,407 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2088,64 +2710,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="39" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="79" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="38" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="78" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="37" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="77" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="36" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="76" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="35" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="75" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="34" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="74" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="33" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="73" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="32" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="72" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="31" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="71" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="30" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="70" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="29" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="69" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="28" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="68" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="27" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="26" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="25" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="65" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="24" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="64" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="23" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="63" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="22" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="62" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="21" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="61" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="20" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="60" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3076,40 +3698,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F6 F10:F100">
-    <cfRule type="top10" dxfId="19" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="59" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G100">
-    <cfRule type="top10" dxfId="18" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="58" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="17" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="57" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="16" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="56" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="15" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="55" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="14" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="54" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="top10" dxfId="13" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="53" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="top10" dxfId="12" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="52" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N1048576 N1:N15">
-    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O1048576 O1:O15">
-    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="50" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F9">
-    <cfRule type="top10" dxfId="9" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="49" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
-    <cfRule type="top10" dxfId="8" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="48" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3121,8 +3743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3316,28 +3938,658 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2">
+    <cfRule type="top10" dxfId="47" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="top10" dxfId="46" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="top10" dxfId="45" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="top10" dxfId="44" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="top10" dxfId="43" priority="4" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="top10" dxfId="42" priority="3" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="top10" dxfId="41" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="top10" dxfId="40" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A67CF49-60A7-4BB0-98FE-FEFDC2499A21}">
+  <dimension ref="A1:AI8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="V2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AF2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI2" s="1"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7.4066000000000001</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.63539999999999996</v>
+      </c>
+      <c r="D4" s="5">
+        <v>10.474399999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.65310000000000001</v>
+      </c>
+      <c r="G4" s="5">
+        <v>10.6031</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.66990000000000005</v>
+      </c>
+      <c r="I4" s="5">
+        <v>10.6135</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.62450000000000006</v>
+      </c>
+      <c r="L4" s="5">
+        <v>7.4286000000000003</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="N4" s="5">
+        <v>8.6626999999999992</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.63470000000000004</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>9.0976999999999997</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.66410000000000002</v>
+      </c>
+      <c r="S4" s="5">
+        <v>8.5055999999999994</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="V4" s="5">
+        <v>10.119899999999999</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0.69669999999999999</v>
+      </c>
+      <c r="X4" s="5">
+        <v>13.149800000000001</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0.61729999999999996</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>9.9131999999999998</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>0.68410000000000004</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>9.2276000000000007</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>0.65649999999999997</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>8.9060000000000006</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0.67149999999999999</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>9.8470999999999993</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0.63959999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="5">
+        <v>10.702500000000001</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.65590000000000004</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8.8918999999999997</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.72040000000000004</v>
+      </c>
+      <c r="G5" s="5">
+        <v>14.615399999999999</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.6603</v>
+      </c>
+      <c r="I5" s="5">
+        <v>11.255599999999999</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="L5" s="5">
+        <v>17.767099999999999</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="N5" s="5">
+        <v>14.950100000000001</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.83709999999999996</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>14.001799999999999</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="S5" s="5">
+        <v>14.4094</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0.76580000000000004</v>
+      </c>
+      <c r="V5" s="5">
+        <v>15.747199999999999</v>
+      </c>
+      <c r="W5" s="5">
+        <v>0.66830000000000001</v>
+      </c>
+      <c r="X5" s="5">
+        <v>15.0436</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0.81230000000000002</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>14.087</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>0.70569999999999999</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>12.7296</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>0.72929999999999995</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>13.9473</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>0.6744</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>12.305300000000001</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>0.76839999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="5">
+        <v>12.343999999999999</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="D6" s="5">
+        <v>11.3879</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.73309999999999997</v>
+      </c>
+      <c r="G6" s="5">
+        <v>14.785299999999999</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.67159999999999997</v>
+      </c>
+      <c r="I6" s="5">
+        <v>12.533300000000001</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.75609999999999999</v>
+      </c>
+      <c r="L6" s="5">
+        <v>15.989699999999999</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.69730000000000003</v>
+      </c>
+      <c r="N6" s="5">
+        <v>16.459900000000001</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.72019999999999995</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>15.406700000000001</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.67490000000000006</v>
+      </c>
+      <c r="S6" s="5">
+        <v>15.6153</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="V6" s="5">
+        <v>15.4777</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0.69140000000000001</v>
+      </c>
+      <c r="X6" s="5">
+        <v>18.6999</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0.77480000000000004</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>14.6221</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>0.71030000000000004</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>12.7278</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>0.74719999999999998</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>14.5943</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>0.68740000000000001</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>13.883800000000001</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>0.75439999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="5">
+        <v>19.4085</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.87019999999999997</v>
+      </c>
+      <c r="D7" s="5">
+        <v>13.601800000000001</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.82769999999999999</v>
+      </c>
+      <c r="G7" s="5">
+        <v>18.085000000000001</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.84350000000000003</v>
+      </c>
+      <c r="I7" s="5">
+        <v>14.511100000000001</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.79469999999999996</v>
+      </c>
+      <c r="L7" s="5">
+        <v>21.516200000000001</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0.8821</v>
+      </c>
+      <c r="N7" s="5">
+        <v>16.944500000000001</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0.8921</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>18.621300000000002</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0.85970000000000002</v>
+      </c>
+      <c r="S7" s="5">
+        <v>17.202200000000001</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="V7" s="5">
+        <v>25.419799999999999</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0.89480000000000004</v>
+      </c>
+      <c r="X7" s="5">
+        <v>22.729099999999999</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>0.87219999999999998</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>18.791</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>14.2422</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>0.81110000000000004</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>19.7285</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>0.86919999999999997</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>15.706099999999999</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>0.83409999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="top10" dxfId="39" priority="28" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="top10" dxfId="38" priority="27" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="top10" dxfId="37" priority="26" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="top10" dxfId="36" priority="25" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3">
+    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3">
+    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3">
+    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3">
+    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3">
+    <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3">
+    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3">
+    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3">
+    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3">
+    <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC3">
     <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="AD3">
     <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+  <conditionalFormatting sqref="AA3">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI3">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG3">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Checkpoint for GTA benchmarking
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D870AF2-EEAC-49CF-A102-2A2B19DC3851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE35AB-0393-4BDB-82F8-870A6E66BB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="162">
   <si>
     <t>PSNR</t>
   </si>
@@ -930,7 +930,147 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="94">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2710,64 +2850,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="79" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="93" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="78" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="92" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="77" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="91" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="76" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="90" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="75" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="89" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="74" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="88" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="73" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="87" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="72" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="86" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="71" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="85" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="70" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="84" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="69" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="83" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="68" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="82" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="67" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="81" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="66" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="80" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="65" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="79" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="64" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="78" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="63" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="77" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="62" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="76" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="61" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="75" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="60" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="74" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3698,40 +3838,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F6 F10:F100">
-    <cfRule type="top10" dxfId="59" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="73" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G100">
-    <cfRule type="top10" dxfId="58" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="72" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="57" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="71" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="56" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="70" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="55" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="69" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="54" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="68" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="top10" dxfId="53" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="top10" dxfId="52" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N1048576 N1:N15">
-    <cfRule type="top10" dxfId="51" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="65" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O1048576 O1:O15">
-    <cfRule type="top10" dxfId="50" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="64" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F9">
-    <cfRule type="top10" dxfId="49" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="63" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
-    <cfRule type="top10" dxfId="48" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="62" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3938,28 +4078,28 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="top10" dxfId="47" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="61" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="46" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="60" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="45" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="59" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="top10" dxfId="44" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="58" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="43" priority="4" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="57" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="42" priority="3" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="56" priority="3" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="41" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="55" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="40" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="54" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3969,10 +4109,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A67CF49-60A7-4BB0-98FE-FEFDC2499A21}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD36" sqref="AD36:AE36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4506,89 +4646,221 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="top10" dxfId="39" priority="28" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="53" priority="42" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="top10" dxfId="38" priority="27" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="52" priority="41" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="top10" dxfId="37" priority="26" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="51" priority="40" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="top10" dxfId="36" priority="25" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="50" priority="39" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="38" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="37" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="35" priority="36" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="35" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="34" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="33" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="31" priority="32" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="30" priority="31" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="30" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="29" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
+    <cfRule type="top10" dxfId="27" priority="28" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="top10" dxfId="26" priority="27" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3">
+    <cfRule type="top10" dxfId="25" priority="26" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3">
+    <cfRule type="top10" dxfId="24" priority="25" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3">
+    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3">
+    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC3">
+    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD3">
+    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA3">
+    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3">
+    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3">
+    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI3">
+    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3">
+    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG3">
+    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
     <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3">
+  <conditionalFormatting sqref="C10">
     <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3">
-    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3">
-    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3">
+  <conditionalFormatting sqref="G10">
+    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10">
     <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3">
+  <conditionalFormatting sqref="M10">
     <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3">
-    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD3">
-    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA3">
+  <conditionalFormatting sqref="Q10">
+    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10">
+    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V10">
     <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3">
+  <conditionalFormatting sqref="W10">
     <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF3">
+  <conditionalFormatting sqref="AA10">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB10">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10">
     <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG3">
+  <conditionalFormatting sqref="AG10">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created checkpoint for no albedo style training.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779AC01F-7DBB-4626-BE7E-1FB66BE8EF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2875B00C-30C6-4E21-B7A3-383773971206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId2"/>
     <sheet name="Maps 2 RGB" sheetId="9" r:id="rId3"/>
-    <sheet name="GTA V Images" sheetId="10" r:id="rId4"/>
+    <sheet name="GTA V Images - RRL" sheetId="10" r:id="rId4"/>
+    <sheet name="GTA V Images - Ours" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -329,8 +330,193 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neil Patrick  A. Del Gallego</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{2621C454-C4CC-45F9-9A57-987ED1BAC695}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{1A7332AB-EBEF-4A0A-BFA0-D4CD3DC6EA69}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{D085DB8D-4CB3-4224-AECA-7AF5D03B9B18}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{E05967C4-0535-42EF-AD04-8D55D37ABD82}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{E6BD1AC0-FC1E-4428-B010-DD9DB222D37B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{19E54573-458B-451C-B9A8-5B75B75A7774}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{D6DE8AF3-AC4D-43E1-AC82-B36D0E32BCD9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check image-specific reconstruction, not RGB.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="171">
   <si>
     <t>PSNR</t>
   </si>
@@ -840,6 +1026,9 @@
   </si>
   <si>
     <t>V4.02.8</t>
+  </si>
+  <si>
+    <t>OURS</t>
   </si>
 </sst>
 </file>
@@ -954,7 +1143,427 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="132">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2834,64 +3443,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="89" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="131" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="88" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="130" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="87" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="129" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="86" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="128" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="85" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="127" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="84" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="126" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="83" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="125" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="82" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="124" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="81" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="123" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="80" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="122" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="79" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="121" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="78" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="120" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="77" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="119" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="76" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="118" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="75" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="117" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="74" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="116" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="73" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="115" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="72" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="114" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="71" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="113" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="70" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="112" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3822,40 +4431,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F6 F10:F100">
-    <cfRule type="top10" dxfId="69" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="111" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G100">
-    <cfRule type="top10" dxfId="68" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="110" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="67" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="109" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="66" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="108" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="65" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="107" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="64" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="106" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="top10" dxfId="63" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="105" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="top10" dxfId="62" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="104" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N1048576 N1:N15">
-    <cfRule type="top10" dxfId="61" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="103" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O1048576 O1:O15">
-    <cfRule type="top10" dxfId="60" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="102" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F9">
-    <cfRule type="top10" dxfId="59" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="101" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
-    <cfRule type="top10" dxfId="58" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="100" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3867,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4390,52 +4999,52 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="top10" dxfId="57" priority="16" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="99" priority="16" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="56" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="98" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="55" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="97" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="top10" dxfId="54" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="96" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="53" priority="12" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="95" priority="12" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="52" priority="11" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="94" priority="11" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="51" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="93" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="50" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="92" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="49" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="91" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="48" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="90" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="47" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="89" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="46" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="88" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="45" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="87" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="44" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="86" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="43" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="85" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="42" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="84" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4447,8 +5056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A67CF49-60A7-4BB0-98FE-FEFDC2499A21}">
   <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,26 +5586,14 @@
       <c r="A8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="5">
-        <v>8.2411999999999992</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.64659999999999995</v>
-      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="G8" s="5">
-        <v>8.343</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="I8" s="5">
-        <v>8.1175999999999995</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.70920000000000005</v>
-      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -5090,133 +5687,642 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="top10" dxfId="41" priority="42" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="83" priority="42" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="top10" dxfId="40" priority="41" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="82" priority="41" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="top10" dxfId="39" priority="40" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="81" priority="40" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="top10" dxfId="38" priority="39" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="80" priority="39" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="top10" dxfId="37" priority="38" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="79" priority="38" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="top10" dxfId="36" priority="37" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="78" priority="37" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="top10" dxfId="35" priority="36" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="77" priority="36" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="top10" dxfId="34" priority="35" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="76" priority="35" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="top10" dxfId="33" priority="34" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="75" priority="34" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="top10" dxfId="32" priority="33" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="74" priority="33" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="top10" dxfId="31" priority="32" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="73" priority="32" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="top10" dxfId="30" priority="31" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="72" priority="31" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="top10" dxfId="29" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="71" priority="30" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="top10" dxfId="28" priority="29" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="70" priority="29" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="top10" dxfId="27" priority="28" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="69" priority="28" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="top10" dxfId="26" priority="27" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="68" priority="27" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="top10" dxfId="25" priority="26" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="26" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3">
-    <cfRule type="top10" dxfId="24" priority="25" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="25" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3">
-    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="65" priority="24" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3">
-    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="64" priority="23" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3">
-    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="63" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD3">
-    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="62" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3">
-    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="61" priority="20" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="60" priority="19" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3">
-    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="59" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="58" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3">
-    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="57" priority="16" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG3">
-    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="56" priority="15" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="55" priority="14" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="54" priority="13" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="53" priority="12" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="52" priority="11" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="51" priority="10" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="50" priority="9" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="49" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="48" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="47" priority="6" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="5" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="45" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="44" priority="3" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="43" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG10">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="42" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF40BC5-E637-4A9D-AFCD-CD414A7F8E77}">
+  <dimension ref="A1:AI14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="V2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AF2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI2" s="1"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4.8019999999999996</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.5867</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="5">
+        <v>7.0015000000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.62019999999999997</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="L4" s="5">
+        <v>6.6082000000000001</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.62580000000000002</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="Q4" s="5">
+        <v>5.7142999999999997</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="V4">
+        <v>5.3742999999999999</v>
+      </c>
+      <c r="W4">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="AA4" s="5">
+        <v>5.9706000000000001</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>0.60229999999999995</v>
+      </c>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AF4" s="5">
+        <v>6.4029999999999996</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0.61050000000000004</v>
+      </c>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AF9" s="1"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="top10" dxfId="41" priority="42" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="top10" dxfId="40" priority="41" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="top10" dxfId="39" priority="40" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="top10" dxfId="38" priority="39" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="top10" dxfId="37" priority="38" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="top10" dxfId="36" priority="37" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="top10" dxfId="35" priority="36" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="top10" dxfId="34" priority="35" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="top10" dxfId="33" priority="34" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3">
+    <cfRule type="top10" dxfId="32" priority="33" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3">
+    <cfRule type="top10" dxfId="31" priority="32" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="top10" dxfId="30" priority="31" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3">
+    <cfRule type="top10" dxfId="29" priority="30" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3">
+    <cfRule type="top10" dxfId="28" priority="29" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3">
+    <cfRule type="top10" dxfId="27" priority="28" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="top10" dxfId="26" priority="27" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3">
+    <cfRule type="top10" dxfId="25" priority="26" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3">
+    <cfRule type="top10" dxfId="24" priority="25" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3">
+    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3">
+    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC3">
+    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD3">
+    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA3">
+    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3">
+    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3">
+    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI3">
+    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3">
+    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG3">
+    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10">
+    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M10">
+    <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q10">
+    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10">
+    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V10">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W10">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA10">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB10">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG10">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for no albedo training.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2875B00C-30C6-4E21-B7A3-383773971206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3268B2DF-53F5-4F54-B94C-AD0268804D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,7 +336,7 @@
     <author>Neil Patrick  A. Del Gallego</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{2621C454-C4CC-45F9-9A57-987ED1BAC695}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{D6DE8AF3-AC4D-43E1-AC82-B36D0E32BCD9}">
       <text>
         <r>
           <rPr>
@@ -361,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{1A7332AB-EBEF-4A0A-BFA0-D4CD3DC6EA69}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{2621C454-C4CC-45F9-9A57-987ED1BAC695}">
       <text>
         <r>
           <rPr>
@@ -386,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{D085DB8D-4CB3-4224-AECA-7AF5D03B9B18}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{1A7332AB-EBEF-4A0A-BFA0-D4CD3DC6EA69}">
       <text>
         <r>
           <rPr>
@@ -411,7 +411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{E05967C4-0535-42EF-AD04-8D55D37ABD82}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{D085DB8D-4CB3-4224-AECA-7AF5D03B9B18}">
       <text>
         <r>
           <rPr>
@@ -436,7 +436,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{E6BD1AC0-FC1E-4428-B010-DD9DB222D37B}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{E05967C4-0535-42EF-AD04-8D55D37ABD82}">
       <text>
         <r>
           <rPr>
@@ -461,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{19E54573-458B-451C-B9A8-5B75B75A7774}">
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{E6BD1AC0-FC1E-4428-B010-DD9DB222D37B}">
       <text>
         <r>
           <rPr>
@@ -486,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{D6DE8AF3-AC4D-43E1-AC82-B36D0E32BCD9}">
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{19E54573-458B-451C-B9A8-5B75B75A7774}">
       <text>
         <r>
           <rPr>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="177">
   <si>
     <t>PSNR</t>
   </si>
@@ -1029,6 +1029,24 @@
   </si>
   <si>
     <t>OURS</t>
+  </si>
+  <si>
+    <t>V4.05.5</t>
+  </si>
+  <si>
+    <t>V4.05.6</t>
+  </si>
+  <si>
+    <t>V4.04.5</t>
+  </si>
+  <si>
+    <t>V4.04.6</t>
+  </si>
+  <si>
+    <t>V4.04.7</t>
+  </si>
+  <si>
+    <t>V4.04.8</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1139,11 +1157,982 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="132">
+  <dxfs count="229">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3443,64 +4432,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="131" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="228" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="130" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="227" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="129" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="226" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="128" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="225" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="127" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="224" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="126" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="223" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="125" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="222" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="124" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="221" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="123" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="220" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="122" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="219" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="121" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="218" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="120" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="217" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="119" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="216" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="118" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="215" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="117" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="214" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="116" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="213" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="115" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="212" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="114" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="211" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="113" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="210" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="112" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="209" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4431,40 +5420,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F6 F10:F100">
-    <cfRule type="top10" dxfId="111" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="208" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G100">
-    <cfRule type="top10" dxfId="110" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="207" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="109" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="206" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="108" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="205" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="107" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="204" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="106" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="203" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="top10" dxfId="105" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="202" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="top10" dxfId="104" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="201" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N1048576 N1:N15">
-    <cfRule type="top10" dxfId="103" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="200" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O1048576 O1:O15">
-    <cfRule type="top10" dxfId="102" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="199" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F9">
-    <cfRule type="top10" dxfId="101" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="198" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
-    <cfRule type="top10" dxfId="100" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="197" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4474,10 +5463,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4996,55 +5985,205 @@
         <v>0.76449999999999996</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="5">
+        <v>11.966200000000001</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.77180000000000004</v>
+      </c>
+      <c r="D19" s="5">
+        <v>14.827999999999999</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.79549999999999998</v>
+      </c>
+      <c r="F19" s="5">
+        <v>16.446000000000002</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="H19" s="5">
+        <v>22.953600000000002</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0.92230000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="5">
+        <v>11.9511</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.73609999999999998</v>
+      </c>
+      <c r="D20" s="5">
+        <v>12.814399999999999</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.80730000000000002</v>
+      </c>
+      <c r="F20" s="5">
+        <v>19.706099999999999</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.8286</v>
+      </c>
+      <c r="H20" s="5">
+        <v>28.9803</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0.95820000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="5">
+        <v>11.4352</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.78569999999999995</v>
+      </c>
+      <c r="D21" s="5">
+        <v>13.806800000000001</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.81469999999999998</v>
+      </c>
+      <c r="F21" s="5">
+        <v>18.768699999999999</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.84019999999999995</v>
+      </c>
+      <c r="H21" s="5">
+        <v>25.644300000000001</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0.93149999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="5">
+        <v>11.0627</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.74560000000000004</v>
+      </c>
+      <c r="D22" s="5">
+        <v>14.251300000000001</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.78920000000000001</v>
+      </c>
+      <c r="F22" s="5">
+        <v>10.612</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="H22" s="5">
+        <v>21.146899999999999</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0.89690000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="5">
+        <v>12.297800000000001</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.76170000000000004</v>
+      </c>
+      <c r="D23" s="5">
+        <v>17.347899999999999</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.82169999999999999</v>
+      </c>
+      <c r="F23" s="5">
+        <v>18.777899999999999</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.81020000000000003</v>
+      </c>
+      <c r="H23" s="5">
+        <v>29.309899999999999</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0.96589999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="5">
+        <v>11.434200000000001</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="D24" s="5">
+        <v>15.6431</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.81030000000000002</v>
+      </c>
+      <c r="F24" s="5">
+        <v>18.504799999999999</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.81230000000000002</v>
+      </c>
+      <c r="H24" s="5">
+        <v>30.055499999999999</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0.96020000000000005</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="top10" dxfId="99" priority="16" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="98" priority="15" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="97" priority="14" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
-    <cfRule type="top10" dxfId="96" priority="13" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="95" priority="12" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="94" priority="11" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="93" priority="10" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="92" priority="9" percent="1" rank="10"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="91" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="90" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="89" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="88" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="87" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="86" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="85" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="84" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5687,130 +6826,130 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="top10" dxfId="83" priority="42" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="196" priority="42" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="top10" dxfId="82" priority="41" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="195" priority="41" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="top10" dxfId="81" priority="40" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="194" priority="40" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="top10" dxfId="80" priority="39" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="193" priority="39" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="top10" dxfId="79" priority="38" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="192" priority="38" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="top10" dxfId="78" priority="37" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="191" priority="37" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="top10" dxfId="77" priority="36" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="190" priority="36" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="top10" dxfId="76" priority="35" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="189" priority="35" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="top10" dxfId="75" priority="34" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="188" priority="34" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="top10" dxfId="74" priority="33" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="187" priority="33" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="top10" dxfId="73" priority="32" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="186" priority="32" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="top10" dxfId="72" priority="31" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="185" priority="31" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="top10" dxfId="71" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="184" priority="30" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="top10" dxfId="70" priority="29" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="183" priority="29" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="top10" dxfId="69" priority="28" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="182" priority="28" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="top10" dxfId="68" priority="27" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="181" priority="27" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="top10" dxfId="67" priority="26" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="180" priority="26" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3">
-    <cfRule type="top10" dxfId="66" priority="25" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="179" priority="25" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3">
-    <cfRule type="top10" dxfId="65" priority="24" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="178" priority="24" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3">
-    <cfRule type="top10" dxfId="64" priority="23" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="177" priority="23" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3">
-    <cfRule type="top10" dxfId="63" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="176" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD3">
-    <cfRule type="top10" dxfId="62" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="175" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3">
-    <cfRule type="top10" dxfId="61" priority="20" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="174" priority="20" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="top10" dxfId="60" priority="19" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="173" priority="19" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3">
-    <cfRule type="top10" dxfId="59" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="172" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="top10" dxfId="58" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="171" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3">
-    <cfRule type="top10" dxfId="57" priority="16" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="170" priority="16" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG3">
-    <cfRule type="top10" dxfId="56" priority="15" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="169" priority="15" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="top10" dxfId="55" priority="14" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="168" priority="14" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="top10" dxfId="54" priority="13" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="167" priority="13" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="top10" dxfId="53" priority="12" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="166" priority="12" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="top10" dxfId="52" priority="11" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="165" priority="11" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="top10" dxfId="51" priority="10" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="164" priority="10" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="top10" dxfId="50" priority="9" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="163" priority="9" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="top10" dxfId="49" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="162" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="top10" dxfId="48" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="161" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="top10" dxfId="47" priority="6" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="160" priority="6" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10">
-    <cfRule type="top10" dxfId="46" priority="5" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="159" priority="5" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="top10" dxfId="45" priority="4" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="158" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10">
-    <cfRule type="top10" dxfId="44" priority="3" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="157" priority="3" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10">
-    <cfRule type="top10" dxfId="43" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="156" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG10">
-    <cfRule type="top10" dxfId="42" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="155" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5820,45 +6959,45 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF40BC5-E637-4A9D-AFCD-CD414A7F8E77}">
-  <dimension ref="A1:AI14"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="10" width="11.42578125" customWidth="1"/>
+    <col min="2" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>123</v>
       </c>
@@ -5866,6 +7005,7 @@
         <v>122</v>
       </c>
       <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>123</v>
       </c>
@@ -5909,7 +7049,7 @@
       </c>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -5922,6 +7062,7 @@
       <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="8" t="s">
         <v>0</v>
       </c>
@@ -5995,331 +7136,250 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>166</v>
       </c>
       <c r="B4" s="5">
-        <v>4.8019999999999996</v>
+        <v>6.4029999999999996</v>
       </c>
       <c r="C4" s="5">
-        <v>0.5867</v>
+        <v>0.61050000000000004</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5">
-        <v>7.0015000000000001</v>
+        <v>4.8019999999999996</v>
       </c>
       <c r="H4" s="5">
-        <v>0.62019999999999997</v>
+        <v>0.5867</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="L4" s="5">
-        <v>6.6082000000000001</v>
+        <v>7.0015000000000001</v>
       </c>
       <c r="M4" s="5">
-        <v>0.62580000000000002</v>
+        <v>0.62019999999999997</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="Q4" s="5">
-        <v>5.7142999999999997</v>
+        <v>6.6082000000000001</v>
       </c>
       <c r="R4" s="5">
-        <v>0.58720000000000006</v>
+        <v>0.62580000000000002</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="V4">
-        <v>5.3742999999999999</v>
-      </c>
-      <c r="W4">
-        <v>0.59399999999999997</v>
+      <c r="V4" s="5">
+        <v>5.7142999999999997</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0.58720000000000006</v>
       </c>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="AA4" s="5">
-        <v>5.9706000000000001</v>
-      </c>
-      <c r="AB4" s="5">
-        <v>0.60229999999999995</v>
+      <c r="AA4">
+        <v>5.3742999999999999</v>
+      </c>
+      <c r="AB4">
+        <v>0.59399999999999997</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AF4" s="5">
-        <v>6.4029999999999996</v>
+        <v>5.9706000000000001</v>
       </c>
       <c r="AG4" s="5">
-        <v>0.61050000000000004</v>
+        <v>0.60229999999999995</v>
       </c>
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+        <v>173</v>
+      </c>
+      <c r="B5" s="5">
+        <v>6.6196000000000002</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.66990000000000005</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="K5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="V5" s="5"/>
+      <c r="U5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="AA5" s="5"/>
+      <c r="Z5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
-      <c r="AF5" s="5"/>
+      <c r="AE5" s="5"/>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="5"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+        <v>174</v>
+      </c>
+      <c r="B6" s="5">
+        <v>6.4764999999999997</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.66669999999999996</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="K6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="V6" s="5"/>
+      <c r="U6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
-      <c r="AA6" s="5"/>
+      <c r="Z6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
-      <c r="AF6" s="5"/>
+      <c r="AE6" s="5"/>
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="5"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="B7" s="5">
+        <v>7.0194999999999999</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.66820000000000002</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="P7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="V7" s="5"/>
+      <c r="U7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-      <c r="AA7" s="5"/>
+      <c r="Z7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
-      <c r="AF7" s="5"/>
+      <c r="AE7" s="5"/>
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="AJ7" s="5"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="5">
+        <v>6.4603999999999999</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.66339999999999999</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="7">
+        <v>6.5223000000000004</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.64939999999999998</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="14">
+        <v>6.4854000000000003</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.65529999999999999</v>
+      </c>
       <c r="H10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="I10" s="8"/>
       <c r="M10" s="8"/>
-      <c r="Q10" s="8"/>
+      <c r="N10" s="8"/>
       <c r="R10" s="8"/>
-      <c r="V10" s="8"/>
+      <c r="S10" s="8"/>
       <c r="W10" s="8"/>
-      <c r="AA10" s="8"/>
+      <c r="X10" s="8"/>
       <c r="AB10" s="8"/>
-      <c r="AF10" s="8"/>
+      <c r="AC10" s="8"/>
       <c r="AG10" s="8"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH10" s="8"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="top10" dxfId="41" priority="42" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="top10" dxfId="40" priority="41" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="top10" dxfId="39" priority="40" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="top10" dxfId="38" priority="39" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="top10" dxfId="37" priority="38" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3">
-    <cfRule type="top10" dxfId="36" priority="37" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="top10" dxfId="35" priority="36" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="top10" dxfId="34" priority="35" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
-    <cfRule type="top10" dxfId="33" priority="34" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="top10" dxfId="32" priority="33" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3">
-    <cfRule type="top10" dxfId="31" priority="32" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3">
-    <cfRule type="top10" dxfId="30" priority="31" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3">
-    <cfRule type="top10" dxfId="29" priority="30" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3">
-    <cfRule type="top10" dxfId="28" priority="29" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3">
-    <cfRule type="top10" dxfId="27" priority="28" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R3">
-    <cfRule type="top10" dxfId="26" priority="27" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3">
-    <cfRule type="top10" dxfId="25" priority="26" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3">
-    <cfRule type="top10" dxfId="24" priority="25" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3">
-    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3">
-    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC3">
-    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD3">
-    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA3">
-    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB3">
-    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH3">
-    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
-    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF3">
-    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG3">
-    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L10">
-    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q10">
-    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R10">
-    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V10">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W10">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA10">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB10">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF10">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG10">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="top10" dxfId="70" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="top10" dxfId="68" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Bug fixes. Fixed seed to promote reproducibility.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3268B2DF-53F5-4F54-B94C-AD0268804D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF45D76-3500-4D47-9E3F-B9F08680A009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="1470" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="181">
   <si>
     <t>PSNR</t>
   </si>
@@ -1047,6 +1047,18 @@
   </si>
   <si>
     <t>V4.04.8</t>
+  </si>
+  <si>
+    <t>V4.06.5</t>
+  </si>
+  <si>
+    <t>V4.06.6</t>
+  </si>
+  <si>
+    <t>V4.06.7</t>
+  </si>
+  <si>
+    <t>V4.06.8</t>
   </si>
 </sst>
 </file>
@@ -1154,1465 +1166,15 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="229">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="84">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3771,38 +2333,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="K1" s="13" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="13"/>
+      <c r="L1" s="14"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="13"/>
+      <c r="O1" s="14"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4432,64 +2994,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="228" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="83" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="227" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="82" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="226" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="81" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="225" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="80" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="224" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="79" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="223" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="78" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="222" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="77" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="221" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="76" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="220" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="75" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="219" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="74" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="218" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="73" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="217" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="72" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="216" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="71" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="215" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="70" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="214" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="69" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="213" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="68" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="212" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="211" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="210" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="65" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="209" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="64" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5420,40 +3982,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F6 F10:F100">
-    <cfRule type="top10" dxfId="208" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="63" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G100">
-    <cfRule type="top10" dxfId="207" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="62" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="206" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="61" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="205" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="60" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="204" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="59" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="203" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="58" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="top10" dxfId="202" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="57" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="top10" dxfId="201" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="56" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N1048576 N1:N15">
-    <cfRule type="top10" dxfId="200" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="55" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O1048576 O1:O15">
-    <cfRule type="top10" dxfId="199" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="54" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F9">
-    <cfRule type="top10" dxfId="198" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="53" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
-    <cfRule type="top10" dxfId="197" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="52" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5463,10 +4025,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6159,31 +4721,99 @@
         <v>0.96020000000000005</v>
       </c>
     </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="5">
+        <v>17.706900000000001</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.76649999999999996</v>
+      </c>
+      <c r="D25" s="5">
+        <v>19.653099999999998</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.86029999999999995</v>
+      </c>
+      <c r="F25" s="5">
+        <v>22.648900000000001</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.90410000000000001</v>
+      </c>
+      <c r="H25" s="5">
+        <v>21.154800000000002</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0.85070000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="5">
+        <v>17.365400000000001</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.76890000000000003</v>
+      </c>
+      <c r="D26" s="5">
+        <v>19.2791</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.85189999999999999</v>
+      </c>
+      <c r="F26" s="5">
+        <v>23.146000000000001</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.90639999999999998</v>
+      </c>
+      <c r="H26" s="5">
+        <v>22.748899999999999</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0.86929999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="14" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="51" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="13" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="50" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="12" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="49" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="11" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="48" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="10" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="47" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="9" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="8" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="45" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="44" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6826,130 +5456,130 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="top10" dxfId="196" priority="42" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="42" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="top10" dxfId="195" priority="41" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="41" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="top10" dxfId="194" priority="40" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="41" priority="40" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="top10" dxfId="193" priority="39" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="40" priority="39" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="top10" dxfId="192" priority="38" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="39" priority="38" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="top10" dxfId="191" priority="37" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="37" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="top10" dxfId="190" priority="36" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="37" priority="36" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="top10" dxfId="189" priority="35" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="36" priority="35" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="top10" dxfId="188" priority="34" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="34" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="top10" dxfId="187" priority="33" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="33" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="top10" dxfId="186" priority="32" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="33" priority="32" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="top10" dxfId="185" priority="31" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="31" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="top10" dxfId="184" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="30" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="top10" dxfId="183" priority="29" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="29" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="top10" dxfId="182" priority="28" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="28" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="top10" dxfId="181" priority="27" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="27" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="top10" dxfId="180" priority="26" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="26" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3">
-    <cfRule type="top10" dxfId="179" priority="25" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="25" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3">
-    <cfRule type="top10" dxfId="178" priority="24" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="24" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3">
-    <cfRule type="top10" dxfId="177" priority="23" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="23" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3">
-    <cfRule type="top10" dxfId="176" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD3">
-    <cfRule type="top10" dxfId="175" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3">
-    <cfRule type="top10" dxfId="174" priority="20" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="20" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="top10" dxfId="173" priority="19" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="19" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3">
-    <cfRule type="top10" dxfId="172" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="top10" dxfId="171" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3">
-    <cfRule type="top10" dxfId="170" priority="16" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="16" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG3">
-    <cfRule type="top10" dxfId="169" priority="15" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="15" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="top10" dxfId="168" priority="14" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="14" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="top10" dxfId="167" priority="13" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="13" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="top10" dxfId="166" priority="12" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="12" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="top10" dxfId="165" priority="11" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="11" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="top10" dxfId="164" priority="10" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="10" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="top10" dxfId="163" priority="9" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="9" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="top10" dxfId="162" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="top10" dxfId="161" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="top10" dxfId="160" priority="6" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10">
-    <cfRule type="top10" dxfId="159" priority="5" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="top10" dxfId="158" priority="4" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10">
-    <cfRule type="top10" dxfId="157" priority="3" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="3" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10">
-    <cfRule type="top10" dxfId="156" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG10">
-    <cfRule type="top10" dxfId="155" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7351,10 +5981,10 @@
       <c r="A10" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>6.4854000000000003</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>0.65529999999999999</v>
       </c>
       <c r="H10" s="8"/>
@@ -7376,10 +6006,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="70" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="68" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Bu g fixes in albedo training.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF45D76-3500-4D47-9E3F-B9F08680A009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B3DBAA-8579-4AE4-A467-BC988F0B23B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="1470" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="185">
   <si>
     <t>PSNR</t>
   </si>
@@ -1059,6 +1059,18 @@
   </si>
   <si>
     <t>V4.06.8</t>
+  </si>
+  <si>
+    <t>V4.07.5</t>
+  </si>
+  <si>
+    <t>V4.07.6</t>
+  </si>
+  <si>
+    <t>V4.07.7</t>
+  </si>
+  <si>
+    <t>V4.07.8</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1081,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1117,6 +1129,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1150,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1170,6 +1189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4025,10 +4045,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,28 +4745,28 @@
       <c r="A25" t="s">
         <v>177</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="15">
         <v>17.706900000000001</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="15">
         <v>0.76649999999999996</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="15">
         <v>19.653099999999998</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="15">
         <v>0.86029999999999995</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="15">
         <v>22.648900000000001</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="15">
         <v>0.90410000000000001</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="15">
         <v>21.154800000000002</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="15">
         <v>0.85070000000000001</v>
       </c>
     </row>
@@ -4754,28 +4774,28 @@
       <c r="A26" t="s">
         <v>178</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="15">
         <v>17.365400000000001</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="15">
         <v>0.76890000000000003</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="15">
         <v>19.2791</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="15">
         <v>0.85189999999999999</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="15">
         <v>23.146000000000001</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="15">
         <v>0.90639999999999998</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="15">
         <v>22.748899999999999</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="15">
         <v>0.86929999999999996</v>
       </c>
     </row>
@@ -4783,10 +4803,102 @@
       <c r="A27" t="s">
         <v>179</v>
       </c>
+      <c r="B27" s="15">
+        <v>12.3668</v>
+      </c>
+      <c r="C27" s="15">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="D27" s="15">
+        <v>18.418500000000002</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0.84709999999999996</v>
+      </c>
+      <c r="F27" s="15">
+        <v>22.5608</v>
+      </c>
+      <c r="G27" s="15">
+        <v>0.86829999999999996</v>
+      </c>
+      <c r="H27" s="15">
+        <v>16.315799999999999</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0.82110000000000005</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>180</v>
+      </c>
+      <c r="B28" s="15">
+        <v>15.368399999999999</v>
+      </c>
+      <c r="C28" s="15">
+        <v>0.74960000000000004</v>
+      </c>
+      <c r="D28" s="15">
+        <v>19.710999999999999</v>
+      </c>
+      <c r="E28" s="15">
+        <v>0.877</v>
+      </c>
+      <c r="F28" s="15">
+        <v>23.2363</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0.88929999999999998</v>
+      </c>
+      <c r="H28" s="15">
+        <v>20.630400000000002</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0.87549999999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="15">
+        <v>18.610700000000001</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0.79330000000000001</v>
+      </c>
+      <c r="D29" s="15">
+        <v>20.399799999999999</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.88759999999999994</v>
+      </c>
+      <c r="F29" s="15">
+        <v>20.9389</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="H29" s="15">
+        <v>25.526199999999999</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0.91520000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix on OOM slurm error
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640BFDDE-24E2-4E7D-BFEB-74DBC3D65570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E85576-BAB0-48D1-98F0-D50CCEB0F2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="1875" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="209">
   <si>
     <t>PSNR</t>
   </si>
@@ -1095,6 +1095,54 @@
   </si>
   <si>
     <t>V4.13.12</t>
+  </si>
+  <si>
+    <t>V4.08.5</t>
+  </si>
+  <si>
+    <t>V4.08.6</t>
+  </si>
+  <si>
+    <t>V4.08.7</t>
+  </si>
+  <si>
+    <t>V4.08.8</t>
+  </si>
+  <si>
+    <t>V4.08.9</t>
+  </si>
+  <si>
+    <t>V4.08.10</t>
+  </si>
+  <si>
+    <t>V4.08.11</t>
+  </si>
+  <si>
+    <t>V4.08.12</t>
+  </si>
+  <si>
+    <t>V4.09.5</t>
+  </si>
+  <si>
+    <t>V4.09.6</t>
+  </si>
+  <si>
+    <t>V4.09.7</t>
+  </si>
+  <si>
+    <t>V4.09.8</t>
+  </si>
+  <si>
+    <t>V4.09.9</t>
+  </si>
+  <si>
+    <t>V4.09.10</t>
+  </si>
+  <si>
+    <t>V4.09.11</t>
+  </si>
+  <si>
+    <t>V4.09.12</t>
   </si>
 </sst>
 </file>
@@ -4061,10 +4109,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,7 +4123,7 @@
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4991,233 +5040,505 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>185</v>
-      </c>
-      <c r="B33" s="11">
-        <v>7.6628999999999996</v>
-      </c>
-      <c r="C33" s="11">
-        <v>0.68859999999999999</v>
-      </c>
-      <c r="D33" s="11">
-        <v>21.343499999999999</v>
-      </c>
-      <c r="E33" s="11">
-        <v>0.92010000000000003</v>
-      </c>
-      <c r="F33" s="11">
-        <v>20.311699999999998</v>
-      </c>
-      <c r="G33" s="11">
-        <v>0.87960000000000005</v>
-      </c>
-      <c r="H33" s="11">
-        <v>25.898700000000002</v>
-      </c>
-      <c r="I33" s="11">
-        <v>0.93620000000000003</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" s="11">
-        <v>7.0274999999999999</v>
-      </c>
-      <c r="C34" s="11">
-        <v>0.66220000000000001</v>
-      </c>
-      <c r="D34" s="11">
-        <v>20.7424</v>
-      </c>
-      <c r="E34" s="11">
-        <v>0.91459999999999997</v>
-      </c>
-      <c r="F34" s="11">
-        <v>18.465599999999998</v>
-      </c>
-      <c r="G34" s="11">
-        <v>0.86519999999999997</v>
-      </c>
-      <c r="H34" s="11">
-        <v>25.020299999999999</v>
-      </c>
-      <c r="I34" s="11">
-        <v>0.92549999999999999</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>187</v>
-      </c>
-      <c r="B35" s="11">
-        <v>6.3823999999999996</v>
-      </c>
-      <c r="C35" s="11">
-        <v>0.65149999999999997</v>
-      </c>
-      <c r="D35" s="11">
-        <v>20.296099999999999</v>
-      </c>
-      <c r="E35" s="11">
-        <v>0.91369999999999996</v>
-      </c>
-      <c r="F35" s="11">
-        <v>19.272500000000001</v>
-      </c>
-      <c r="G35" s="11">
-        <v>0.87309999999999999</v>
-      </c>
-      <c r="H35" s="11">
-        <v>25.5596</v>
-      </c>
-      <c r="I35" s="11">
-        <v>0.93459999999999999</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>188</v>
-      </c>
-      <c r="B36" s="11">
-        <v>5.0491000000000001</v>
-      </c>
-      <c r="C36" s="11">
-        <v>0.62190000000000001</v>
-      </c>
-      <c r="D36" s="11">
-        <v>19</v>
-      </c>
-      <c r="E36" s="11">
-        <v>0.9042</v>
-      </c>
-      <c r="F36" s="11">
-        <v>14.5</v>
-      </c>
-      <c r="G36" s="11">
-        <v>0.81159999999999999</v>
-      </c>
-      <c r="H36" s="11">
-        <v>23.5486</v>
-      </c>
-      <c r="I36" s="11">
-        <v>0.90839999999999999</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>189</v>
-      </c>
-      <c r="B37" s="11">
-        <v>8.6103000000000005</v>
-      </c>
-      <c r="C37" s="11">
-        <v>0.65280000000000005</v>
-      </c>
-      <c r="D37" s="11">
-        <v>21.138999999999999</v>
-      </c>
-      <c r="E37" s="11">
-        <v>0.88619999999999999</v>
-      </c>
-      <c r="F37" s="11">
-        <v>24.367699999999999</v>
-      </c>
-      <c r="G37" s="11">
-        <v>0.92949999999999999</v>
-      </c>
-      <c r="H37" s="11">
-        <v>22.5031</v>
-      </c>
-      <c r="I37" s="11">
-        <v>0.86040000000000005</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B38" s="11">
-        <v>8.1295999999999999</v>
-      </c>
-      <c r="C38" s="11">
-        <v>0.65690000000000004</v>
-      </c>
-      <c r="D38" s="11">
-        <v>21.4176</v>
-      </c>
-      <c r="E38" s="11">
-        <v>0.89049999999999996</v>
-      </c>
-      <c r="F38" s="11">
-        <v>24.453800000000001</v>
-      </c>
-      <c r="G38" s="11">
-        <v>0.93220000000000003</v>
-      </c>
-      <c r="H38" s="11">
-        <v>24.329599999999999</v>
-      </c>
-      <c r="I38" s="11">
-        <v>0.90149999999999997</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B39" s="11">
-        <v>8.1849000000000007</v>
-      </c>
-      <c r="C39" s="11">
-        <v>0.66759999999999997</v>
-      </c>
-      <c r="D39" s="11">
-        <v>21.020099999999999</v>
-      </c>
-      <c r="E39" s="11">
-        <v>0.87749999999999995</v>
-      </c>
-      <c r="F39" s="11">
-        <v>24.7698</v>
-      </c>
-      <c r="G39" s="11">
-        <v>0.93279999999999996</v>
-      </c>
-      <c r="H39" s="11">
-        <v>24.911200000000001</v>
-      </c>
-      <c r="I39" s="11">
-        <v>0.89980000000000004</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="11">
+        <v>7.0720999999999998</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0.62690000000000001</v>
+      </c>
+      <c r="D41" s="11">
+        <v>14.2727</v>
+      </c>
+      <c r="E41" s="11">
+        <v>0.76419999999999999</v>
+      </c>
+      <c r="F41" s="11">
+        <v>16.8795</v>
+      </c>
+      <c r="G41" s="11">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="H41" s="11">
+        <v>21.4055</v>
+      </c>
+      <c r="I41" s="11">
+        <v>0.82389999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="11">
+        <v>7.3131000000000004</v>
+      </c>
+      <c r="C42" s="11">
+        <v>0.58889999999999998</v>
+      </c>
+      <c r="D42" s="11">
+        <v>13.1126</v>
+      </c>
+      <c r="E42" s="11">
+        <v>0.71289999999999998</v>
+      </c>
+      <c r="F42" s="11">
+        <v>16.585799999999999</v>
+      </c>
+      <c r="G42" s="11">
+        <v>0.80010000000000003</v>
+      </c>
+      <c r="H42" s="11">
+        <v>17.6601</v>
+      </c>
+      <c r="I42" s="11">
+        <v>0.74490000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="11">
+        <v>6.7933000000000003</v>
+      </c>
+      <c r="C43" s="11">
+        <v>0.60780000000000001</v>
+      </c>
+      <c r="D43" s="11">
+        <v>14.385400000000001</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0.83379999999999999</v>
+      </c>
+      <c r="F43" s="11">
+        <v>17.566299999999998</v>
+      </c>
+      <c r="G43" s="11">
+        <v>0.82130000000000003</v>
+      </c>
+      <c r="H43" s="11">
+        <v>18.174600000000002</v>
+      </c>
+      <c r="I43" s="11">
+        <v>0.85350000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="11">
+        <v>6.5248999999999997</v>
+      </c>
+      <c r="C44" s="11">
+        <v>0.57040000000000002</v>
+      </c>
+      <c r="D44" s="11">
+        <v>13.501099999999999</v>
+      </c>
+      <c r="E44" s="11">
+        <v>0.78549999999999998</v>
+      </c>
+      <c r="F44" s="11">
+        <v>17.060099999999998</v>
+      </c>
+      <c r="G44" s="11">
+        <v>0.82089999999999996</v>
+      </c>
+      <c r="H44" s="11">
+        <v>18.083100000000002</v>
+      </c>
+      <c r="I44" s="11">
+        <v>0.76529999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>205</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>206</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="11">
+        <v>7.6628999999999996</v>
+      </c>
+      <c r="C49" s="11">
+        <v>0.68859999999999999</v>
+      </c>
+      <c r="D49" s="11">
+        <v>21.343499999999999</v>
+      </c>
+      <c r="E49" s="11">
+        <v>0.92010000000000003</v>
+      </c>
+      <c r="F49" s="11">
+        <v>20.311699999999998</v>
+      </c>
+      <c r="G49" s="11">
+        <v>0.87960000000000005</v>
+      </c>
+      <c r="H49" s="11">
+        <v>25.898700000000002</v>
+      </c>
+      <c r="I49" s="11">
+        <v>0.93620000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="11">
+        <v>7.0274999999999999</v>
+      </c>
+      <c r="C50" s="11">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D50" s="11">
+        <v>20.7424</v>
+      </c>
+      <c r="E50" s="11">
+        <v>0.91459999999999997</v>
+      </c>
+      <c r="F50" s="11">
+        <v>18.465599999999998</v>
+      </c>
+      <c r="G50" s="11">
+        <v>0.86519999999999997</v>
+      </c>
+      <c r="H50" s="11">
+        <v>25.020299999999999</v>
+      </c>
+      <c r="I50" s="11">
+        <v>0.92549999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>187</v>
+      </c>
+      <c r="B51" s="11">
+        <v>6.3823999999999996</v>
+      </c>
+      <c r="C51" s="11">
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="D51" s="11">
+        <v>20.296099999999999</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0.91369999999999996</v>
+      </c>
+      <c r="F51" s="11">
+        <v>19.272500000000001</v>
+      </c>
+      <c r="G51" s="11">
+        <v>0.87309999999999999</v>
+      </c>
+      <c r="H51" s="11">
+        <v>25.5596</v>
+      </c>
+      <c r="I51" s="11">
+        <v>0.93459999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="11">
+        <v>5.0491000000000001</v>
+      </c>
+      <c r="C52" s="11">
+        <v>0.62190000000000001</v>
+      </c>
+      <c r="D52" s="11">
+        <v>19</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0.9042</v>
+      </c>
+      <c r="F52" s="11">
+        <v>14.5</v>
+      </c>
+      <c r="G52" s="11">
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="H52" s="11">
+        <v>23.5486</v>
+      </c>
+      <c r="I52" s="11">
+        <v>0.90839999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" s="11">
+        <v>8.6103000000000005</v>
+      </c>
+      <c r="C53" s="11">
+        <v>0.65280000000000005</v>
+      </c>
+      <c r="D53" s="11">
+        <v>21.138999999999999</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="F53" s="11">
+        <v>24.367699999999999</v>
+      </c>
+      <c r="G53" s="11">
+        <v>0.92949999999999999</v>
+      </c>
+      <c r="H53" s="11">
+        <v>22.5031</v>
+      </c>
+      <c r="I53" s="11">
+        <v>0.86040000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" s="11">
+        <v>8.1295999999999999</v>
+      </c>
+      <c r="C54" s="11">
+        <v>0.65690000000000004</v>
+      </c>
+      <c r="D54" s="11">
+        <v>21.4176</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0.89049999999999996</v>
+      </c>
+      <c r="F54" s="11">
+        <v>24.453800000000001</v>
+      </c>
+      <c r="G54" s="11">
+        <v>0.93220000000000003</v>
+      </c>
+      <c r="H54" s="11">
+        <v>24.329599999999999</v>
+      </c>
+      <c r="I54" s="11">
+        <v>0.90149999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" s="11">
+        <v>8.1849000000000007</v>
+      </c>
+      <c r="C55" s="11">
+        <v>0.66759999999999997</v>
+      </c>
+      <c r="D55" s="11">
+        <v>21.020099999999999</v>
+      </c>
+      <c r="E55" s="11">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="F55" s="11">
+        <v>24.7698</v>
+      </c>
+      <c r="G55" s="11">
+        <v>0.93279999999999996</v>
+      </c>
+      <c r="H55" s="11">
+        <v>24.911200000000001</v>
+      </c>
+      <c r="I55" s="11">
+        <v>0.89980000000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>192</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B56" s="11">
         <v>8.1608000000000001</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C56" s="11">
         <v>0.64149999999999996</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D56" s="11">
         <v>21.1768</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E56" s="11">
         <v>0.87639999999999996</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F56" s="11">
         <v>26.054600000000001</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G56" s="11">
         <v>0.94179999999999997</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H56" s="11">
         <v>21.221900000000002</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I56" s="11">
         <v>0.83909999999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated performance for V4.08.XX
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E85576-BAB0-48D1-98F0-D50CCEB0F2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66790A8-B3BD-4906-BB87-50E7579A0A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1875" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4995" yWindow="1965" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4112,8 +4112,8 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5042,53 +5042,117 @@
       <c r="A33" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
+      <c r="B33" s="11">
+        <v>5.86</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.60440000000000005</v>
+      </c>
+      <c r="D33" s="11">
+        <v>12.8194</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="F33" s="11">
+        <v>14.534000000000001</v>
+      </c>
+      <c r="G33" s="11">
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="H33" s="11">
+        <v>17.504999999999999</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0.81569999999999998</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
+      <c r="B34" s="11">
+        <v>7.0288000000000004</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0.6361</v>
+      </c>
+      <c r="D34" s="11">
+        <v>12.803000000000001</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0.79959999999999998</v>
+      </c>
+      <c r="F34" s="11">
+        <v>14.8584</v>
+      </c>
+      <c r="G34" s="11">
+        <v>0.80179999999999996</v>
+      </c>
+      <c r="H34" s="11">
+        <v>17.394500000000001</v>
+      </c>
+      <c r="I34" s="11">
+        <v>0.83679999999999999</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
+      <c r="B35" s="11">
+        <v>6.2824999999999998</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0.61470000000000002</v>
+      </c>
+      <c r="D35" s="11">
+        <v>13.659800000000001</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0.82269999999999999</v>
+      </c>
+      <c r="F35" s="11">
+        <v>13.672800000000001</v>
+      </c>
+      <c r="G35" s="11">
+        <v>0.77710000000000001</v>
+      </c>
+      <c r="H35" s="11">
+        <v>17.3598</v>
+      </c>
+      <c r="I35" s="11">
+        <v>0.81569999999999998</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>196</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
+      <c r="B36" s="11">
+        <v>6.4057000000000004</v>
+      </c>
+      <c r="C36" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="D36" s="11">
+        <v>13.8142</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0.8196</v>
+      </c>
+      <c r="F36" s="11">
+        <v>14.1731</v>
+      </c>
+      <c r="G36" s="11">
+        <v>0.77769999999999995</v>
+      </c>
+      <c r="H36" s="11">
+        <v>17.474599999999999</v>
+      </c>
+      <c r="I36" s="11">
+        <v>0.81830000000000003</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">

</xml_diff>

<commit_message>
Documented performances. Fixed hyperparameters
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D42965A-081C-484F-92A6-B57C018D5767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4CC917-6743-42CF-B1A4-6450BB3464CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="1245" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="352">
   <si>
     <t>PSNR</t>
   </si>
@@ -1488,6 +1488,93 @@
   </si>
   <si>
     <t>V8.04.18</t>
+  </si>
+  <si>
+    <t>REVISE hyperparameters</t>
+  </si>
+  <si>
+    <t>V9.00.05</t>
+  </si>
+  <si>
+    <t>V9.00.06</t>
+  </si>
+  <si>
+    <t>V9.00.07</t>
+  </si>
+  <si>
+    <t>V9.00.08</t>
+  </si>
+  <si>
+    <t>V9.00.09</t>
+  </si>
+  <si>
+    <t>V9.00.10</t>
+  </si>
+  <si>
+    <t>V9.00.11</t>
+  </si>
+  <si>
+    <t>V9.00.12</t>
+  </si>
+  <si>
+    <t>V9.00.13</t>
+  </si>
+  <si>
+    <t>V9.00.14</t>
+  </si>
+  <si>
+    <t>V9.00.15</t>
+  </si>
+  <si>
+    <t>V9.00.16</t>
+  </si>
+  <si>
+    <t>V9.00.17</t>
+  </si>
+  <si>
+    <t>V9.00.18</t>
+  </si>
+  <si>
+    <t>V9.01.5</t>
+  </si>
+  <si>
+    <t>V9.01.6</t>
+  </si>
+  <si>
+    <t>V9.01.7</t>
+  </si>
+  <si>
+    <t>V9.01.8</t>
+  </si>
+  <si>
+    <t>V9.01.9</t>
+  </si>
+  <si>
+    <t>V9.01.10</t>
+  </si>
+  <si>
+    <t>V9.01.11</t>
+  </si>
+  <si>
+    <t>V9.01.12</t>
+  </si>
+  <si>
+    <t>V9.01.13</t>
+  </si>
+  <si>
+    <t>V9.01.14</t>
+  </si>
+  <si>
+    <t>V9.01.15</t>
+  </si>
+  <si>
+    <t>V9.01.16</t>
+  </si>
+  <si>
+    <t>V9.01.17</t>
+  </si>
+  <si>
+    <t>V9.01.18</t>
   </si>
 </sst>
 </file>
@@ -4455,11 +4542,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:I169"/>
+  <dimension ref="A1:J197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B156" sqref="B156:I157"/>
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7904,7 +7991,7 @@
         <v>0.86070000000000002</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>298</v>
       </c>
@@ -7933,7 +8020,7 @@
         <v>0.78669999999999995</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>299</v>
       </c>
@@ -7962,22 +8049,22 @@
         <v>0.85940000000000005</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>303</v>
       </c>
@@ -8006,7 +8093,7 @@
         <v>0.85070000000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>304</v>
       </c>
@@ -8035,7 +8122,7 @@
         <v>0.85670000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>305</v>
       </c>
@@ -8064,7 +8151,7 @@
         <v>0.84250000000000003</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>306</v>
       </c>
@@ -8093,7 +8180,7 @@
         <v>0.86070000000000002</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>307</v>
       </c>
@@ -8122,7 +8209,7 @@
         <v>0.8548</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>308</v>
       </c>
@@ -8151,7 +8238,7 @@
         <v>0.85550000000000004</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>309</v>
       </c>
@@ -8180,7 +8267,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>310</v>
       </c>
@@ -8209,7 +8296,7 @@
         <v>0.72789999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>311</v>
       </c>
@@ -8237,8 +8324,11 @@
       <c r="I158" s="4">
         <v>0.69350000000000001</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>312</v>
       </c>
@@ -8266,8 +8356,11 @@
       <c r="I159" s="4">
         <v>0.67449999999999999</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>313</v>
       </c>
@@ -8295,8 +8388,11 @@
       <c r="I160" s="4">
         <v>0.67769999999999997</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J160" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>314</v>
       </c>
@@ -8324,8 +8420,11 @@
       <c r="I161" s="4">
         <v>0.66069999999999995</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J161" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>315</v>
       </c>
@@ -8354,7 +8453,7 @@
         <v>0.66649999999999998</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>316</v>
       </c>
@@ -8383,7 +8482,7 @@
         <v>0.68320000000000003</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>317</v>
       </c>
@@ -8412,7 +8511,7 @@
         <v>0.63726000000000005</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>318</v>
       </c>
@@ -8441,7 +8540,7 @@
         <v>0.65990000000000004</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>319</v>
       </c>
@@ -8470,7 +8569,7 @@
         <v>0.63900000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>320</v>
       </c>
@@ -8499,7 +8598,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>321</v>
       </c>
@@ -8528,7 +8627,7 @@
         <v>0.65280000000000005</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>322</v>
       </c>
@@ -8555,6 +8654,242 @@
       </c>
       <c r="I169" s="4">
         <v>0.66249999999999998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>324</v>
+      </c>
+      <c r="B170" s="4">
+        <v>4.484</v>
+      </c>
+      <c r="C170" s="4">
+        <v>0.5474</v>
+      </c>
+      <c r="D170" s="4">
+        <v>6.5403000000000002</v>
+      </c>
+      <c r="E170" s="4">
+        <v>0.69010000000000005</v>
+      </c>
+      <c r="F170" s="4">
+        <v>9.4009999999999998</v>
+      </c>
+      <c r="G170" s="4">
+        <v>0.73629999999999995</v>
+      </c>
+      <c r="H170" s="4">
+        <v>12.702</v>
+      </c>
+      <c r="I170" s="4">
+        <v>0.79690000000000005</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>325</v>
+      </c>
+      <c r="B171" s="4">
+        <v>4.5608000000000004</v>
+      </c>
+      <c r="C171" s="4">
+        <v>0.54510000000000003</v>
+      </c>
+      <c r="D171" s="4">
+        <v>6.3360000000000003</v>
+      </c>
+      <c r="E171" s="4">
+        <v>0.68710000000000004</v>
+      </c>
+      <c r="F171" s="4">
+        <v>9.3574000000000002</v>
+      </c>
+      <c r="G171" s="4">
+        <v>0.73980000000000001</v>
+      </c>
+      <c r="H171" s="4">
+        <v>13.037000000000001</v>
+      </c>
+      <c r="I171" s="4">
+        <v>0.81140000000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>334</v>
+      </c>
+      <c r="B180" s="4">
+        <v>4.8554000000000004</v>
+      </c>
+      <c r="C180" s="4">
+        <v>0.5464</v>
+      </c>
+      <c r="D180" s="4">
+        <v>6.4715999999999996</v>
+      </c>
+      <c r="E180" s="4">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F180" s="4">
+        <v>8.7712000000000003</v>
+      </c>
+      <c r="G180" s="4">
+        <v>0.74050000000000005</v>
+      </c>
+      <c r="H180" s="4">
+        <v>13.092700000000001</v>
+      </c>
+      <c r="I180" s="4">
+        <v>0.81910000000000005</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>335</v>
+      </c>
+      <c r="B181" s="4">
+        <v>4.6875999999999998</v>
+      </c>
+      <c r="C181" s="4">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="D181" s="4">
+        <v>6.1853999999999996</v>
+      </c>
+      <c r="E181" s="4">
+        <v>0.68440000000000001</v>
+      </c>
+      <c r="F181" s="4">
+        <v>8.6862999999999992</v>
+      </c>
+      <c r="G181" s="4">
+        <v>0.73280000000000001</v>
+      </c>
+      <c r="H181" s="4">
+        <v>13.4095</v>
+      </c>
+      <c r="I181" s="4">
+        <v>0.82294</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logged metrics for V9.07.XX
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52015538-B45C-426B-99AF-858601490629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6373A5-5315-481F-B28D-B3657BB381DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="1245" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="366">
   <si>
     <t>PSNR</t>
   </si>
@@ -1575,6 +1575,48 @@
   </si>
   <si>
     <t>V9.01.18</t>
+  </si>
+  <si>
+    <t>V9.07.5</t>
+  </si>
+  <si>
+    <t>V9.07.6</t>
+  </si>
+  <si>
+    <t>V9.07.7</t>
+  </si>
+  <si>
+    <t>V9.07.8</t>
+  </si>
+  <si>
+    <t>V9.07.9</t>
+  </si>
+  <si>
+    <t>V9.07.10</t>
+  </si>
+  <si>
+    <t>V9.07.11</t>
+  </si>
+  <si>
+    <t>V9.07.12</t>
+  </si>
+  <si>
+    <t>V9.07.13</t>
+  </si>
+  <si>
+    <t>V9.07.14</t>
+  </si>
+  <si>
+    <t>V9.07.15</t>
+  </si>
+  <si>
+    <t>V9.07.16</t>
+  </si>
+  <si>
+    <t>V9.07.17</t>
+  </si>
+  <si>
+    <t>V9.07.18</t>
   </si>
 </sst>
 </file>
@@ -4542,11 +4584,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:J197"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F196" sqref="F196"/>
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I188" sqref="I188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8860,41 +8902,233 @@
       <c r="A186" t="s">
         <v>340</v>
       </c>
+      <c r="B186" s="4">
+        <v>15.470800000000001</v>
+      </c>
+      <c r="C186" s="4">
+        <v>0.82089999999999996</v>
+      </c>
+      <c r="D186" s="4">
+        <v>8.3193000000000001</v>
+      </c>
+      <c r="E186" s="4">
+        <v>0.72419999999999995</v>
+      </c>
+      <c r="F186" s="4">
+        <v>15.119</v>
+      </c>
+      <c r="G186" s="4">
+        <v>0.80179999999999996</v>
+      </c>
+      <c r="H186" s="4">
+        <v>21.343900000000001</v>
+      </c>
+      <c r="I186" s="4">
+        <v>0.79920000000000002</v>
+      </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>341</v>
       </c>
+      <c r="B187" s="4">
+        <v>13.161899999999999</v>
+      </c>
+      <c r="C187" s="4">
+        <v>0.80349999999999999</v>
+      </c>
+      <c r="D187" s="4">
+        <v>8.5847999999999995</v>
+      </c>
+      <c r="E187" s="4">
+        <v>0.72450000000000003</v>
+      </c>
+      <c r="F187" s="4">
+        <v>16.0564</v>
+      </c>
+      <c r="G187" s="4">
+        <v>0.81540000000000001</v>
+      </c>
+      <c r="H187" s="4">
+        <v>21.759399999999999</v>
+      </c>
+      <c r="I187" s="4">
+        <v>0.79649999999999999</v>
+      </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>342</v>
       </c>
+      <c r="B188" s="4">
+        <v>13.1266</v>
+      </c>
+      <c r="C188" s="4">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="D188" s="4">
+        <v>8.7202000000000002</v>
+      </c>
+      <c r="E188" s="4">
+        <v>0.72889999999999999</v>
+      </c>
+      <c r="F188" s="4">
+        <v>16.145600000000002</v>
+      </c>
+      <c r="G188" s="4">
+        <v>0.82020000000000004</v>
+      </c>
+      <c r="H188" s="4">
+        <v>17.914100000000001</v>
+      </c>
+      <c r="I188" s="4">
+        <v>0.78890000000000005</v>
+      </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>343</v>
       </c>
+      <c r="B189" s="4">
+        <v>13.143599999999999</v>
+      </c>
+      <c r="C189" s="4">
+        <v>0.80149999999999999</v>
+      </c>
+      <c r="D189" s="4">
+        <v>8.1607000000000003</v>
+      </c>
+      <c r="E189" s="4">
+        <v>0.73060000000000003</v>
+      </c>
+      <c r="F189" s="4">
+        <v>16.287199999999999</v>
+      </c>
+      <c r="G189" s="4">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="H189" s="4">
+        <v>17.088899999999999</v>
+      </c>
+      <c r="I189" s="4">
+        <v>0.78680000000000005</v>
+      </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>344</v>
       </c>
+      <c r="B190" s="4">
+        <v>13.1805</v>
+      </c>
+      <c r="C190" s="4">
+        <v>0.80079999999999996</v>
+      </c>
+      <c r="D190" s="4">
+        <v>8.3765000000000001</v>
+      </c>
+      <c r="E190" s="4">
+        <v>0.72829999999999995</v>
+      </c>
+      <c r="F190" s="4">
+        <v>15.666700000000001</v>
+      </c>
+      <c r="G190" s="4">
+        <v>0.81669999999999998</v>
+      </c>
+      <c r="H190" s="4">
+        <v>17.705300000000001</v>
+      </c>
+      <c r="I190" s="4">
+        <v>0.79169999999999996</v>
+      </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>345</v>
       </c>
+      <c r="B191" s="4">
+        <v>13.072100000000001</v>
+      </c>
+      <c r="C191" s="4">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="D191" s="4">
+        <v>8.1210000000000004</v>
+      </c>
+      <c r="E191" s="4">
+        <v>0.73280000000000001</v>
+      </c>
+      <c r="F191" s="4">
+        <v>16.355599999999999</v>
+      </c>
+      <c r="G191" s="4">
+        <v>0.83030000000000004</v>
+      </c>
+      <c r="H191" s="4">
+        <v>16.6251</v>
+      </c>
+      <c r="I191" s="4">
+        <v>0.78169999999999995</v>
+      </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>346</v>
       </c>
+      <c r="B192" s="4">
+        <v>13.245100000000001</v>
+      </c>
+      <c r="C192" s="4">
+        <v>0.80079999999999996</v>
+      </c>
+      <c r="D192" s="4">
+        <v>8.2849000000000004</v>
+      </c>
+      <c r="E192" s="4">
+        <v>0.73029999999999995</v>
+      </c>
+      <c r="F192" s="4">
+        <v>14.848800000000001</v>
+      </c>
+      <c r="G192" s="4">
+        <v>0.79659999999999997</v>
+      </c>
+      <c r="H192" s="4">
+        <v>18.8231</v>
+      </c>
+      <c r="I192" s="4">
+        <v>0.79349999999999998</v>
+      </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>347</v>
       </c>
+      <c r="B193" s="4">
+        <v>13.4854</v>
+      </c>
+      <c r="C193" s="4">
+        <v>0.80069999999999997</v>
+      </c>
+      <c r="D193" s="4">
+        <v>8.7506000000000004</v>
+      </c>
+      <c r="E193" s="4">
+        <v>0.73060000000000003</v>
+      </c>
+      <c r="F193" s="4">
+        <v>16.5245</v>
+      </c>
+      <c r="G193" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H193" s="4">
+        <v>18.223199999999999</v>
+      </c>
+      <c r="I193" s="4">
+        <v>0.77980000000000005</v>
+      </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
@@ -8964,31 +9198,101 @@
         <v>351</v>
       </c>
     </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>365</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B56:B121 B123:B140 B142:B184 B197:B1048576 B186:B195 B1:B54">
-    <cfRule type="top10" dxfId="51" priority="8" rank="1"/>
+  <conditionalFormatting sqref="B56:B121 B123:B140 B142:B184 B197:B1048576 B187:B195 B1:B54">
+    <cfRule type="top10" dxfId="51" priority="43" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C121 C123:C140 C142:C184 C197:C1048576 C186:C195 C1:C54">
-    <cfRule type="top10" dxfId="50" priority="7" rank="1"/>
+  <conditionalFormatting sqref="C56:C121 C123:C140 C142:C184 C197:C1048576 C187:C195 C1:C54">
+    <cfRule type="top10" dxfId="50" priority="50" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D121 D123:D140 D142:D184 D197:D1048576 D186:D195 D1:D54">
-    <cfRule type="top10" dxfId="49" priority="6" rank="1"/>
+  <conditionalFormatting sqref="D56:D121 D123:D140 D142:D184 D197:D1048576 D187:D195 D1:D54">
+    <cfRule type="top10" dxfId="49" priority="57" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E121 E123:E140 E142:E184 E197:E1048576 E186:E195 E1:E54">
-    <cfRule type="top10" dxfId="48" priority="5" rank="1"/>
+  <conditionalFormatting sqref="E56:E121 E123:E140 E142:E184 E197:E1048576 E187:E195 E1:E54">
+    <cfRule type="top10" dxfId="48" priority="64" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87:F89 F91 F93:F96 F98:F103 F105:F121 F123:F140 F142:F184 F197:F1048576 F186:F195 H104 H97 H92 H90 F56:F75 F78 F80:F85 H79 H76:H77 H86 F1:F54">
-    <cfRule type="top10" dxfId="47" priority="4" rank="1"/>
+  <conditionalFormatting sqref="F87:F89 F91 F93:F96 F98:F103 F105:F121 F123:F140 F142:F184 F197:F1048576 F187:F195 H104 H97 H92 H90 F56:F75 F78 F80:F85 H79 H76:H77 H86 F1:F54">
+    <cfRule type="top10" dxfId="47" priority="71" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G87:G89 G91 G93:G96 G98:G103 G105:G121 G123:G140 G142:G184 G197:G1048576 G186:G195 I104 I97 I92 I90 G56:G75 G78 G80:G85 I79 I76:I77 I86 G1:G54">
-    <cfRule type="top10" dxfId="46" priority="3" rank="1"/>
+  <conditionalFormatting sqref="G87:G89 G91 G93:G96 G98:G103 G105:G121 G123:G140 G142:G184 G197:G1048576 G187:G195 I104 I97 I92 I90 G56:G75 G78 G80:G85 I79 I76:I77 I86 G1:G54">
+    <cfRule type="top10" dxfId="46" priority="92" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H87:H89 H91 H93:H96 H98:H103 H105:H121 H123:H140 H142:H184 H197:H1048576 H186:H195 H56:H75 H78 H80:H85 H1:H54">
-    <cfRule type="top10" dxfId="45" priority="2" rank="1"/>
+  <conditionalFormatting sqref="H87:H89 H91 H93:H96 H98:H103 H105:H121 H123:H140 H142:H184 H197:H1048576 H187:H195 H56:H75 H78 H80:H85 H1:H54">
+    <cfRule type="top10" dxfId="45" priority="113" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I89 I91 I93:I96 I98:I103 I105:I121 I123:I140 I142:I184 I197:I1048576 I186:I195 I56:I75 I78 I80:I85 I1:I54">
-    <cfRule type="top10" dxfId="44" priority="1" rank="1"/>
+  <conditionalFormatting sqref="I87:I89 I91 I93:I96 I98:I103 I105:I121 I123:I140 I142:I184 I197:I1048576 I187:I195 I56:I75 I78 I80:I85 I1:I54">
+    <cfRule type="top10" dxfId="44" priority="127" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparation for V10.XX.XX experiment
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0B48FF-DDFE-49D0-B82B-048AACCCE5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E02BDC-9748-40CA-AA5E-7EDA69884C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="1245" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="382">
   <si>
     <t>PSNR</t>
   </si>
@@ -1623,6 +1623,48 @@
   </si>
   <si>
     <t>WHDR to beat</t>
+  </si>
+  <si>
+    <t>V10.07.5</t>
+  </si>
+  <si>
+    <t>V10.07.6</t>
+  </si>
+  <si>
+    <t>V10.07.7</t>
+  </si>
+  <si>
+    <t>V10.07.8</t>
+  </si>
+  <si>
+    <t>V10.07.9</t>
+  </si>
+  <si>
+    <t>V10.07.10</t>
+  </si>
+  <si>
+    <t>V10.07.11</t>
+  </si>
+  <si>
+    <t>V10.07.12</t>
+  </si>
+  <si>
+    <t>V10.07.13</t>
+  </si>
+  <si>
+    <t>V10.07.14</t>
+  </si>
+  <si>
+    <t>V10.07.15</t>
+  </si>
+  <si>
+    <t>V10.07.16</t>
+  </si>
+  <si>
+    <t>V10.07.17</t>
+  </si>
+  <si>
+    <t>V10.07.18</t>
   </si>
 </sst>
 </file>
@@ -4590,11 +4632,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:K211"/>
+  <dimension ref="A1:K225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F209" sqref="F209"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H214" sqref="H214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9292,23 +9334,96 @@
       <c r="J208">
         <v>0.44379999999999997</v>
       </c>
-      <c r="K208">
+      <c r="K208" s="1">
         <v>0.21</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>378</v>
+      </c>
+      <c r="J222">
+        <v>0.43580000000000002</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkpoint for V11.XX.XX training
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E02BDC-9748-40CA-AA5E-7EDA69884C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F588635-A832-40EE-A0D1-C0C77DE6D30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="1245" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4635,8 +4635,8 @@
   <dimension ref="A1:K225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H214" sqref="H214"/>
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H223" sqref="H223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9406,6 +9406,30 @@
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>378</v>
+      </c>
+      <c r="B222" s="4">
+        <v>15.171900000000001</v>
+      </c>
+      <c r="C222" s="4">
+        <v>0.80520000000000003</v>
+      </c>
+      <c r="D222" s="4">
+        <v>16.747399999999999</v>
+      </c>
+      <c r="E222" s="4">
+        <v>0.8639</v>
+      </c>
+      <c r="F222" s="4">
+        <v>22.553899999999999</v>
+      </c>
+      <c r="G222" s="4">
+        <v>0.81640000000000001</v>
+      </c>
+      <c r="H222" s="4">
+        <v>24.244499999999999</v>
+      </c>
+      <c r="I222" s="4">
+        <v>0.8871</v>
       </c>
       <c r="J222">
         <v>0.43580000000000002</v>

</xml_diff>

<commit_message>
Bug fixes and optimization for V11.XX.XX
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F588635-A832-40EE-A0D1-C0C77DE6D30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54721B22-630B-4573-AF05-0E45AE3BA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="1245" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="1680" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Maps 2 RGB'!$B$1:$I$74</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -519,7 +520,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="396">
   <si>
     <t>PSNR</t>
   </si>
@@ -1665,6 +1666,48 @@
   </si>
   <si>
     <t>V10.07.18</t>
+  </si>
+  <si>
+    <t>V11.07.15</t>
+  </si>
+  <si>
+    <t>V11.07.5</t>
+  </si>
+  <si>
+    <t>V11.07.6</t>
+  </si>
+  <si>
+    <t>V11.07.7</t>
+  </si>
+  <si>
+    <t>V11.07.8</t>
+  </si>
+  <si>
+    <t>V11.07.9</t>
+  </si>
+  <si>
+    <t>V11.07.10</t>
+  </si>
+  <si>
+    <t>V11.07.11</t>
+  </si>
+  <si>
+    <t>V11.07.12</t>
+  </si>
+  <si>
+    <t>V11.07.13</t>
+  </si>
+  <si>
+    <t>V11.07.14</t>
+  </si>
+  <si>
+    <t>V11.07.16</t>
+  </si>
+  <si>
+    <t>V11.07.17</t>
+  </si>
+  <si>
+    <t>V11.07.18</t>
   </si>
 </sst>
 </file>
@@ -4632,11 +4675,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:K225"/>
+  <dimension ref="A1:K239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H223" sqref="H223"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J226" sqref="J226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9445,9 +9488,157 @@
         <v>380</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>383</v>
+      </c>
+      <c r="B226" s="4">
+        <v>16.901399999999999</v>
+      </c>
+      <c r="C226" s="4">
+        <v>0.84289999999999998</v>
+      </c>
+      <c r="D226" s="4">
+        <v>18.3841</v>
+      </c>
+      <c r="E226" s="4">
+        <v>0.86850000000000005</v>
+      </c>
+      <c r="F226" s="4">
+        <v>19.847200000000001</v>
+      </c>
+      <c r="G226" s="4">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="H226" s="4">
+        <v>22.9116</v>
+      </c>
+      <c r="I226" s="4">
+        <v>0.90049999999999997</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>382</v>
+      </c>
+      <c r="B236" s="4">
+        <v>16.488700000000001</v>
+      </c>
+      <c r="C236" s="4">
+        <v>0.8397</v>
+      </c>
+      <c r="D236" s="4">
+        <v>18.514500000000002</v>
+      </c>
+      <c r="E236" s="4">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="F236" s="4">
+        <v>22.343800000000002</v>
+      </c>
+      <c r="G236" s="4">
+        <v>0.78979999999999995</v>
+      </c>
+      <c r="H236" s="4">
+        <v>25.673100000000002</v>
+      </c>
+      <c r="I236" s="4">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="J236">
+        <v>0.41149999999999998</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>393</v>
+      </c>
+      <c r="B237" s="4">
+        <v>15.151400000000001</v>
+      </c>
+      <c r="C237" s="4">
+        <v>0.81230000000000002</v>
+      </c>
+      <c r="D237" s="4">
+        <v>17.089500000000001</v>
+      </c>
+      <c r="E237" s="4">
+        <v>0.86019999999999996</v>
+      </c>
+      <c r="F237" s="4">
+        <v>20.121600000000001</v>
+      </c>
+      <c r="G237" s="4">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="H237" s="4">
+        <v>23.152899999999999</v>
+      </c>
+      <c r="I237" s="4">
+        <v>0.88560000000000005</v>
+      </c>
+      <c r="J237">
+        <v>0.41830000000000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set RTX 3090 workers back to 12
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FB9318-2F6B-4F08-A27C-33B876ED902C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B656B7F3-C106-41F2-9BD2-8C9672322CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="1680" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1639,7 +1639,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1686,12 +1686,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4614,7 +4608,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A210" sqref="A210"/>
+      <selection pane="bottomLeft" activeCell="I209" sqref="I209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9446,6 +9440,33 @@
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>364</v>
+      </c>
+      <c r="B208" s="4">
+        <v>14.621600000000001</v>
+      </c>
+      <c r="C208" s="4">
+        <v>0.81389999999999996</v>
+      </c>
+      <c r="D208" s="4">
+        <v>18.463699999999999</v>
+      </c>
+      <c r="E208" s="4">
+        <v>0.87919999999999998</v>
+      </c>
+      <c r="F208" s="4">
+        <v>26.3644</v>
+      </c>
+      <c r="G208" s="4">
+        <v>0.81169999999999998</v>
+      </c>
+      <c r="H208" s="4">
+        <v>25.162199999999999</v>
+      </c>
+      <c r="I208" s="4">
+        <v>0.93269999999999997</v>
+      </c>
+      <c r="J208">
+        <v>0.47589999999999999</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactoring cycle gan training
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B656B7F3-C106-41F2-9BD2-8C9672322CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853216E-7F87-4970-A25F-27F182BC8DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="1680" windowWidth="28800" windowHeight="15345" tabRatio="427" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="368">
   <si>
     <t>PSNR</t>
   </si>
@@ -1629,6 +1629,9 @@
   </si>
   <si>
     <t>V13.10.15</t>
+  </si>
+  <si>
+    <t>GTA</t>
   </si>
 </sst>
 </file>
@@ -1749,7 +1752,747 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="158">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3574,64 +4317,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="83" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="157" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="82" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="156" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="81" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="155" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="80" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="154" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="79" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="153" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="78" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="152" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="77" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="151" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="76" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="150" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="75" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="149" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="74" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="148" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="73" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="147" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="72" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="146" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="71" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="145" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="70" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="144" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="69" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="143" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="68" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="142" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="67" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="141" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="66" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="140" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="65" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="139" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="64" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="138" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4561,40 +5304,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F6 F10:F100">
-    <cfRule type="top10" dxfId="63" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="137" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G100">
-    <cfRule type="top10" dxfId="62" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="136" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="61" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="135" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="60" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="134" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B1048576 B1:B45">
-    <cfRule type="top10" dxfId="59" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="133" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C1048576 C1:C45">
-    <cfRule type="top10" dxfId="58" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="132" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="top10" dxfId="57" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="131" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="top10" dxfId="56" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="130" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N1048576 N1:N15">
-    <cfRule type="top10" dxfId="55" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="129" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O1048576 O1:O15">
-    <cfRule type="top10" dxfId="54" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="128" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F9">
-    <cfRule type="top10" dxfId="53" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="127" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
-    <cfRule type="top10" dxfId="52" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="126" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4604,11 +5347,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7FCCD-6DEF-4489-B535-F792B4F2F5DA}">
-  <dimension ref="A1:K210"/>
+  <dimension ref="A1:M210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I209" sqref="I209"/>
+      <pane ySplit="2" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,10 +5359,11 @@
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="9" width="11" style="4" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4643,8 +5387,11 @@
       <c r="K1" s="1" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4669,8 +5416,14 @@
       <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -4699,7 +5452,7 @@
         <v>0.84430000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -4728,7 +5481,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -4757,7 +5510,7 @@
         <v>0.79449999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -4786,7 +5539,7 @@
         <v>0.80120000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -4815,7 +5568,7 @@
         <v>0.7833</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -4844,7 +5597,7 @@
         <v>0.76449999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -4873,7 +5626,7 @@
         <v>0.92230000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -4902,7 +5655,7 @@
         <v>0.95820000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -4931,7 +5684,7 @@
         <v>0.93149999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -4960,7 +5713,7 @@
         <v>0.89690000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -4989,7 +5742,7 @@
         <v>0.96589999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>162</v>
       </c>
@@ -5018,7 +5771,7 @@
         <v>0.96020000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>167</v>
       </c>
@@ -5047,7 +5800,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -9128,7 +9881,7 @@
         <v>0.79349999999999998</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>347</v>
       </c>
@@ -9157,7 +9910,7 @@
         <v>0.77980000000000005</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>348</v>
       </c>
@@ -9186,7 +9939,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>349</v>
       </c>
@@ -9215,7 +9968,7 @@
         <v>0.82789999999999997</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>350</v>
       </c>
@@ -9250,7 +10003,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>353</v>
       </c>
@@ -9282,22 +10035,22 @@
         <v>0.43580000000000002</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>358</v>
       </c>
@@ -9329,7 +10082,7 @@
         <v>0.42399999999999999</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -9361,7 +10114,7 @@
         <v>0.39290000000000003</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>359</v>
       </c>
@@ -9390,17 +10143,17 @@
         <v>0.88560000000000005</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -9432,12 +10185,42 @@
         <v>0.49730000000000002</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B207" s="4">
+        <v>15.537599999999999</v>
+      </c>
+      <c r="C207" s="4">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="D207" s="4">
+        <v>18.468</v>
+      </c>
+      <c r="E207" s="4">
+        <v>0.85980000000000001</v>
+      </c>
+      <c r="F207" s="4">
+        <v>26.277200000000001</v>
+      </c>
+      <c r="G207" s="4">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="H207" s="4">
+        <v>25.037800000000001</v>
+      </c>
+      <c r="I207" s="4">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="L207">
+        <v>15.628299999999999</v>
+      </c>
+      <c r="M207">
+        <v>0.71409999999999996</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>364</v>
       </c>
@@ -9468,42 +10251,120 @@
       <c r="J208">
         <v>0.47589999999999999</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L208">
+        <v>15.2889</v>
+      </c>
+      <c r="M208">
+        <v>0.69910000000000005</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209" s="4">
+        <v>16.067900000000002</v>
+      </c>
+      <c r="C209" s="4">
+        <v>0.80979999999999996</v>
+      </c>
+      <c r="D209" s="4">
+        <v>18.695399999999999</v>
+      </c>
+      <c r="E209" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="F209" s="4">
+        <v>37.2271</v>
+      </c>
+      <c r="G209" s="4">
+        <v>0.95889999999999997</v>
+      </c>
+      <c r="H209" s="4">
+        <v>23.219899999999999</v>
+      </c>
+      <c r="I209" s="4">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="L209">
+        <v>12.6412</v>
+      </c>
+      <c r="M209">
+        <v>0.69769999999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>366</v>
       </c>
+      <c r="B210" s="4">
+        <v>16.587900000000001</v>
+      </c>
+      <c r="C210" s="4">
+        <v>0.77629999999999999</v>
+      </c>
+      <c r="D210" s="4">
+        <v>18.4636</v>
+      </c>
+      <c r="E210" s="4">
+        <v>0.82879999999999998</v>
+      </c>
+      <c r="F210" s="4">
+        <v>37.438000000000002</v>
+      </c>
+      <c r="G210" s="4">
+        <v>0.95669999999999999</v>
+      </c>
+      <c r="H210" s="4">
+        <v>23.247599999999998</v>
+      </c>
+      <c r="I210" s="4">
+        <v>0.80259999999999998</v>
+      </c>
+      <c r="J210">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="L210">
+        <v>13.6571</v>
+      </c>
+      <c r="M210">
+        <v>0.70740000000000003</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B56:B121 B123:B140 B142:B184 B187:B1048576 B1:B54">
-    <cfRule type="top10" dxfId="51" priority="128" rank="1"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="top10" dxfId="20" priority="11" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C121 C123:C140 C142:C184 C187:C1048576 C1:C54">
-    <cfRule type="top10" dxfId="50" priority="135" rank="1"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="top10" dxfId="19" priority="10" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D121 D123:D140 D142:D184 D187:D1048576 D1:D54">
-    <cfRule type="top10" dxfId="49" priority="142" rank="1"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="top10" dxfId="18" priority="9" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E121 E123:E140 E142:E184 E187:E1048576 E1:E54">
-    <cfRule type="top10" dxfId="48" priority="149" rank="1"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="17" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87:F89 F91 F93:F96 F98:F103 F105:F121 F123:F140 F142:F184 F187:F1048576 H104 H97 H92 H90 F56:F75 F78 F80:F85 H79 H76:H77 H86 F1:F54">
-    <cfRule type="top10" dxfId="47" priority="156" rank="1"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="16" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G87:G89 G91 G93:G96 G98:G103 G105:G121 G123:G140 G142:G184 G187:G1048576 I104 I97 I92 I90 G56:G75 G78 G80:G85 I79 I76:I77 I86 G1:G54">
-    <cfRule type="top10" dxfId="46" priority="177" rank="1"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="top10" dxfId="15" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H87:H89 H91 H93:H96 H98:H103 H105:H121 H123:H140 H142:H184 H187:H1048576 H56:H75 H78 H80:H85 H1:H54">
-    <cfRule type="top10" dxfId="45" priority="198" rank="1"/>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="14" priority="5" percent="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I89 I91 I93:I96 I98:I103 I105:I121 I123:I140 I142:I184 I187:I1048576 I56:I75 I78 I80:I85 I1:I54">
-    <cfRule type="top10" dxfId="44" priority="212" rank="1"/>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="top10" dxfId="12" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10146,130 +11007,130 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="top10" dxfId="43" priority="42" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="125" priority="42" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="top10" dxfId="42" priority="41" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="124" priority="41" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="top10" dxfId="41" priority="40" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="123" priority="40" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="top10" dxfId="40" priority="39" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="122" priority="39" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="top10" dxfId="39" priority="38" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="121" priority="38" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="top10" dxfId="38" priority="37" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="120" priority="37" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="top10" dxfId="37" priority="36" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="119" priority="36" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="top10" dxfId="36" priority="35" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="118" priority="35" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="top10" dxfId="35" priority="34" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="117" priority="34" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="top10" dxfId="34" priority="33" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="116" priority="33" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="top10" dxfId="33" priority="32" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="115" priority="32" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="top10" dxfId="32" priority="31" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="114" priority="31" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="top10" dxfId="31" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="113" priority="30" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="top10" dxfId="30" priority="29" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="112" priority="29" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="top10" dxfId="29" priority="28" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="111" priority="28" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="top10" dxfId="28" priority="27" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="110" priority="27" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="top10" dxfId="27" priority="26" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="109" priority="26" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3">
-    <cfRule type="top10" dxfId="26" priority="25" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="108" priority="25" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3">
-    <cfRule type="top10" dxfId="25" priority="24" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="107" priority="24" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3">
-    <cfRule type="top10" dxfId="24" priority="23" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="106" priority="23" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3">
-    <cfRule type="top10" dxfId="23" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="105" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD3">
-    <cfRule type="top10" dxfId="22" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="104" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3">
-    <cfRule type="top10" dxfId="21" priority="20" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="103" priority="20" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="top10" dxfId="20" priority="19" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="102" priority="19" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3">
-    <cfRule type="top10" dxfId="19" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="101" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="top10" dxfId="18" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="100" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3">
-    <cfRule type="top10" dxfId="17" priority="16" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="99" priority="16" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG3">
-    <cfRule type="top10" dxfId="16" priority="15" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="98" priority="15" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="top10" dxfId="15" priority="14" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="97" priority="14" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="top10" dxfId="14" priority="13" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="96" priority="13" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="top10" dxfId="13" priority="12" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="95" priority="12" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="top10" dxfId="12" priority="11" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="94" priority="11" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="top10" dxfId="11" priority="10" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="93" priority="10" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="top10" dxfId="10" priority="9" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="92" priority="9" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="top10" dxfId="9" priority="8" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="91" priority="8" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="top10" dxfId="8" priority="7" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="90" priority="7" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="89" priority="6" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10">
-    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="88" priority="5" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="top10" dxfId="5" priority="4" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="87" priority="4" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10">
-    <cfRule type="top10" dxfId="4" priority="3" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="86" priority="3" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10">
-    <cfRule type="top10" dxfId="3" priority="2" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="85" priority="2" percent="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG10">
-    <cfRule type="top10" dxfId="2" priority="1" percent="1" rank="1"/>
+    <cfRule type="top10" dxfId="84" priority="1" percent="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10696,10 +11557,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="83" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="82" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>